<commit_message>
Added groups to clr_GetADobjects
</commit_message>
<xml_diff>
--- a/GetADobjects/AD_DW_Users table map to .net V4.xlsx
+++ b/GetADobjects/AD_DW_Users table map to .net V4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" tabRatio="625" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" tabRatio="625" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,14 @@
     <sheet name="Computers" sheetId="4" r:id="rId3"/>
     <sheet name="Groups" sheetId="5" r:id="rId4"/>
     <sheet name="Users (2)" sheetId="9" r:id="rId5"/>
-    <sheet name="Groups (2)" sheetId="7" r:id="rId6"/>
-    <sheet name="Computers (2)" sheetId="8" r:id="rId7"/>
+    <sheet name="Computers (2)" sheetId="8" r:id="rId6"/>
+    <sheet name="Groups (2)" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Computers!$A$1:$L$38</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Computers (2)'!$A$1:$L$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Computers (2)'!$A$1:$J$43</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Groups!$A$1:$L$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Groups (2)'!$A$1:$L$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Groups (2)'!$A$1:$J$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Users!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Users (2)'!$A$1:$J$68</definedName>
   </definedNames>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="204">
   <si>
     <t>max_length</t>
   </si>
@@ -644,6 +644,12 @@
   </si>
   <si>
     <t>LogonCount</t>
+  </si>
+  <si>
+    <t>GrpCat</t>
+  </si>
+  <si>
+    <t>GrpScope</t>
   </si>
 </sst>
 </file>
@@ -7006,8 +7012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9230,607 +9236,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" customWidth="1"/>
-    <col min="10" max="10" width="88.140625" customWidth="1"/>
-    <col min="11" max="11" width="45.5703125" customWidth="1"/>
-    <col min="12" max="12" width="44.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="J2" s="1" t="str">
-        <f t="shared" ref="J2:J5" si="0">CONCATENATE("collist[",F2,"] = new TableColDef(""",C2,""", typeof(",B2,"), """,I2,""",",H2,");")</f>
-        <v>collist[0] = new TableColDef("Created", typeof(DateTime), "whenCreated",false);</v>
-      </c>
-      <c r="L2" t="str">
-        <f>CONCATENATE("[",C2,"] [",A2,"] ",E2,",")</f>
-        <v>[Created] [datetime] NULL,</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3">
-        <v>256</v>
-      </c>
-      <c r="E3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="J3" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[1] = new TableColDef("Description", typeof(String), "description",false);</v>
-      </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L9" si="1">CONCATENATE("[",C3,"] [",A3,"](",D3,") ",E3,",")</f>
-        <v>[Description] [nvarchar](256) NULL,</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>128</v>
-      </c>
-      <c r="E4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" s="6">
-        <v>2</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="J4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[2] = new TableColDef("DisplayName", typeof(String), "displayname",false);</v>
-      </c>
-      <c r="L4" t="str">
-        <f t="shared" si="1"/>
-        <v>[DisplayName] [nvarchar](128) NULL,</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>512</v>
-      </c>
-      <c r="E5" t="s">
-        <v>115</v>
-      </c>
-      <c r="F5" s="6">
-        <v>3</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="J5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[3] = new TableColDef("DistinguishedName", typeof(String), "distinguishedname",false);</v>
-      </c>
-      <c r="L5" t="str">
-        <f t="shared" si="1"/>
-        <v>[DistinguishedName] [nvarchar](512) NULL,</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6">
-        <v>256</v>
-      </c>
-      <c r="E6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" s="6">
-        <v>4</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="J6" s="1" t="str">
-        <f>CONCATENATE("collist[",F6,"] = new TableColDef(""",C6,""", typeof(",B6,"), """,I6,""",",H6,");")</f>
-        <v>collist[4] = new TableColDef("EmailAddress", typeof(String), "mail",false);</v>
-      </c>
-      <c r="L6" t="str">
-        <f t="shared" si="1"/>
-        <v>[EmailAddress] [nvarchar](256) NULL,</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7">
-        <v>32</v>
-      </c>
-      <c r="E7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F7" s="6">
-        <v>5</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="J7" s="1" t="str">
-        <f t="shared" ref="J7:J16" si="2">CONCATENATE("collist[",F7,"] = new TableColDef(""",C7,""", typeof(",B7,"), """,I7,""",",H7,");")</f>
-        <v>collist[5] = new TableColDef("GroupCategory", typeof(String), "grouptype",true);</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" ref="K7:K8" si="3">CONCATENATE("row[",F7,"] = group.",I7,";")</f>
-        <v>row[5] = group.grouptype;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D8">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>115</v>
-      </c>
-      <c r="F8" s="6">
-        <v>6</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="J8" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>collist[6] = new TableColDef("GroupScope", typeof(String), "grouptype",true);</v>
-      </c>
-      <c r="K8" t="str">
-        <f t="shared" si="3"/>
-        <v>row[6] = group.grouptype;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" t="s">
-        <v>132</v>
-      </c>
-      <c r="D9">
-        <v>256</v>
-      </c>
-      <c r="E9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F9" s="6">
-        <v>7</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="J9" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>collist[7] = new TableColDef("ManagedBy", typeof(String), "managedby",false);</v>
-      </c>
-      <c r="L9" t="str">
-        <f t="shared" si="1"/>
-        <v>[ManagedBy] [nvarchar](256) NULL,</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>115</v>
-      </c>
-      <c r="F10" s="6">
-        <v>8</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="J10" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>collist[8] = new TableColDef("Modified", typeof(DateTime), "whenChanged",false);</v>
-      </c>
-      <c r="L10" t="str">
-        <f>CONCATENATE("[",C10,"] [",A10,"] ",E10,",")</f>
-        <v>[Modified] [datetime] NULL,</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11">
-        <v>256</v>
-      </c>
-      <c r="E11" t="s">
-        <v>115</v>
-      </c>
-      <c r="F11" s="6">
-        <v>9</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>collist[9] = new TableColDef("Name", typeof(String), "name",false);</v>
-      </c>
-      <c r="L11" t="str">
-        <f t="shared" ref="L11:L13" si="4">CONCATENATE("[",C11,"] [",A11,"](",D11,") ",E11,",")</f>
-        <v>[Name] [nvarchar](256) NULL,</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12">
-        <v>128</v>
-      </c>
-      <c r="E12" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="6">
-        <v>10</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="J12" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>collist[10] = new TableColDef("ObjectCategory", typeof(String), "objectcategory",false);</v>
-      </c>
-      <c r="L12" t="str">
-        <f t="shared" si="4"/>
-        <v>[ObjectCategory] [nvarchar](128) NULL,</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13">
-        <v>64</v>
-      </c>
-      <c r="E13" t="s">
-        <v>115</v>
-      </c>
-      <c r="F13" s="6">
-        <v>11</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="J13" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>collist[11] = new TableColDef("ObjectClass", typeof(String), "SchemaClassName",true);</v>
-      </c>
-      <c r="K13" t="str">
-        <f t="shared" ref="K13:K16" si="5">CONCATENATE("row[",F13,"] = group.",I13,";")</f>
-        <v>row[11] = group.SchemaClassName;</v>
-      </c>
-      <c r="L13" t="str">
-        <f t="shared" si="4"/>
-        <v>[ObjectClass] [nvarchar](64) NULL,</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" t="s">
-        <v>116</v>
-      </c>
-      <c r="F14" s="6">
-        <v>12</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="J14" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>collist[12] = new TableColDef("ObjectGUID", typeof(Guid), "Guid",true);</v>
-      </c>
-      <c r="K14" t="str">
-        <f t="shared" si="5"/>
-        <v>row[12] = group.Guid;</v>
-      </c>
-      <c r="L14" t="str">
-        <f>CONCATENATE("[",C14,"] [",A14,"] ",E14,",")</f>
-        <v>[ObjectGUID] [uniqueidentifier] NOT NULL,</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15">
-        <v>128</v>
-      </c>
-      <c r="E15" t="s">
-        <v>115</v>
-      </c>
-      <c r="F15" s="6">
-        <v>13</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="J15" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>collist[13] = new TableColDef("SamAccountName", typeof(String), "samaccountname",false);</v>
-      </c>
-      <c r="L15" t="str">
-        <f t="shared" ref="L15:L16" si="6">CONCATENATE("[",C15,"] [",A15,"](",D15,") ",E15,",")</f>
-        <v>[SamAccountName] [nvarchar](128) NULL,</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16">
-        <v>128</v>
-      </c>
-      <c r="E16" t="s">
-        <v>115</v>
-      </c>
-      <c r="F16" s="6">
-        <v>14</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="J16" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>collist[14] = new TableColDef("SID", typeof(String), "objectsid",true);</v>
-      </c>
-      <c r="K16" t="str">
-        <f t="shared" si="5"/>
-        <v>row[14] = group.objectsid;</v>
-      </c>
-      <c r="L16" t="str">
-        <f t="shared" si="6"/>
-        <v>[SID] [nvarchar](128) NULL,</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:L16"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L42"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9841,14 +9249,12 @@
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="118" customWidth="1"/>
-    <col min="11" max="11" width="75.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="118" customWidth="1"/>
+    <col min="10" max="10" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>118</v>
       </c>
@@ -9870,23 +9276,17 @@
       <c r="G1" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>88</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="J1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -9905,26 +9305,19 @@
       <c r="G2" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="J2" s="1" t="str">
-        <f>CONCATENATE("collist[",F2,"] = new TableColDefEx(""",C2,""", typeof(",B2,"), """,I2,""",""",G2,""");")</f>
+      <c r="I2" s="1" t="str">
+        <f>CONCATENATE("collist[",F2,"] = new TableColDefEx(""",C2,""", typeof(",B2,"), """,H2,""",""",G2,""");")</f>
         <v>collist[0] = new TableColDefEx("AccountExpirationDate", typeof(DateTime), "accountexpires","filetime");</v>
       </c>
-      <c r="K2" t="str">
-        <f>CONCATENATE("if(computer.",I2," !=null) row[",F2,"] = computer.",I2,";")</f>
-        <v>if(computer.accountexpires !=null) row[0] = computer.accountexpires;</v>
-      </c>
-      <c r="L2" t="str">
+      <c r="J2" t="str">
         <f>CONCATENATE("[",C2,"] [",A2,"] ",E2,",")</f>
         <v>[AccountExpirationDate] [datetime] NULL,</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9943,26 +9336,19 @@
       <c r="G3" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="J3" s="1" t="str">
-        <f t="shared" ref="J3:J42" si="0">CONCATENATE("collist[",F3,"] = new TableColDefEx(""",C3,""", typeof(",B3,"), """,I3,""",""",G3,""");")</f>
+      <c r="I3" s="1" t="str">
+        <f>CONCATENATE("collist[",F3,"] = new TableColDefEx(""",C3,""", typeof(",B3,"), """,H3,""",""",G3,""");")</f>
         <v>collist[1] = new TableColDefEx("AccountLockoutTime", typeof(DateTime), "lockouttime","filetime");</v>
       </c>
-      <c r="K3" t="str">
-        <f>CONCATENATE("if(computer.",I3," !=null) row[",F3,"] = computer.",I3,";")</f>
-        <v>if(computer.lockouttime !=null) row[1] = computer.lockouttime;</v>
-      </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L7" si="1">CONCATENATE("[",C3,"] [",A3,"] ",E3,",")</f>
+      <c r="J3" t="str">
+        <f>CONCATENATE("[",C3,"] [",A3,"] ",E3,",")</f>
         <v>[AccountLockoutTime] [datetime] NULL,</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -9981,26 +9367,19 @@
       <c r="G4" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="J4" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I4" s="1" t="str">
+        <f>CONCATENATE("collist[",F4,"] = new TableColDefEx(""",C4,""", typeof(",B4,"), """,H4,""",""",G4,""");")</f>
         <v>collist[2] = new TableColDefEx("AccountNotDelegated", typeof(Boolean), "NOT_DELEGATED","UAC");</v>
       </c>
-      <c r="K4" t="str">
-        <f>CONCATENATE("row[",F4,"] = ((uac &amp; ",I4,") != 0) ? true : false;")</f>
-        <v>row[2] = ((uac &amp; NOT_DELEGATED) != 0) ? true : false;</v>
-      </c>
-      <c r="L4" t="str">
-        <f t="shared" si="1"/>
+      <c r="J4" t="str">
+        <f>CONCATENATE("[",C4,"] [",A4,"] ",E4,",")</f>
         <v>[AccountNotDelegated] [bit] NULL,</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -10019,26 +9398,19 @@
       <c r="G5" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="H5" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="J5" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I5" s="1" t="str">
+        <f>CONCATENATE("collist[",F5,"] = new TableColDefEx(""",C5,""", typeof(",B5,"), """,H5,""",""",G5,""");")</f>
         <v>collist[3] = new TableColDefEx("AllowReversiblePasswordEncryption", typeof(Boolean), "ENCRYPTED_TEXT_PWD_ALLOWED","UAC");</v>
       </c>
-      <c r="K5" t="str">
-        <f>CONCATENATE("row[",F5,"] = computer.",I5,";")</f>
-        <v>row[3] = computer.ENCRYPTED_TEXT_PWD_ALLOWED;</v>
-      </c>
-      <c r="L5" t="str">
-        <f t="shared" si="1"/>
+      <c r="J5" t="str">
+        <f>CONCATENATE("[",C5,"] [",A5,"] ",E5,",")</f>
         <v>[AllowReversiblePasswordEncryption] [bit] NULL,</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -10057,26 +9429,19 @@
       <c r="G6" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I6" s="15" t="s">
+      <c r="H6" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="J6" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I6" s="1" t="str">
+        <f>CONCATENATE("collist[",F6,"] = new TableColDefEx(""",C6,""", typeof(",B6,"), """,H6,""",""",G6,""");")</f>
         <v>collist[4] = new TableColDefEx("BadLogonCount", typeof(Int32), "badpwdcount","Adprop");</v>
       </c>
-      <c r="K6" t="str">
-        <f t="shared" ref="K6:K7" si="2">CONCATENATE("row[",F6,"] = computer.",I6,";")</f>
-        <v>row[4] = computer.badpwdcount;</v>
-      </c>
-      <c r="L6" t="str">
-        <f t="shared" si="1"/>
+      <c r="J6" t="str">
+        <f>CONCATENATE("[",C6,"] [",A6,"] ",E6,",")</f>
         <v>[BadLogonCount] [int] NULL,</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -10095,26 +9460,19 @@
       <c r="G7" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I7" s="17" t="s">
+      <c r="H7" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="J7" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I7" s="1" t="str">
+        <f>CONCATENATE("collist[",F7,"] = new TableColDefEx(""",C7,""", typeof(",B7,"), """,H7,""",""",G7,""");")</f>
         <v>collist[5] = new TableColDefEx("CannotChangePassword", typeof(Boolean), "PASSWD_CANT_CHANGE","UAC");</v>
       </c>
-      <c r="K7" t="str">
-        <f t="shared" si="2"/>
-        <v>row[5] = computer.PASSWD_CANT_CHANGE;</v>
-      </c>
-      <c r="L7" t="str">
-        <f t="shared" si="1"/>
+      <c r="J7" t="str">
+        <f>CONCATENATE("[",C7,"] [",A7,"] ",E7,",")</f>
         <v>[CannotChangePassword] [bit] NULL,</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -10136,22 +9494,19 @@
       <c r="G8" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I8" s="15" t="s">
+      <c r="H8" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="J8" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I8" s="1" t="str">
+        <f>CONCATENATE("collist[",F8,"] = new TableColDefEx(""",C8,""", typeof(",B8,"), """,H8,""",""",G8,""");")</f>
         <v>collist[6] = new TableColDefEx("CN", typeof(String), "cn","Adprop");</v>
       </c>
-      <c r="L8" t="str">
-        <f t="shared" ref="L8" si="3">CONCATENATE("[",C8,"] [",A8,"](",D8,") ",E8,",")</f>
+      <c r="J8" t="str">
+        <f>CONCATENATE("[",C8,"] [",A8,"](",D8,") ",E8,",")</f>
         <v>[CN] [nvarchar](256) NULL,</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -10170,22 +9525,19 @@
       <c r="G9" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="15" t="s">
+      <c r="H9" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I9" s="1" t="str">
+        <f>CONCATENATE("collist[",F9,"] = new TableColDefEx(""",C9,""", typeof(",B9,"), """,H9,""",""",G9,""");")</f>
         <v>collist[7] = new TableColDefEx("Created", typeof(DateTime), "whenCreated","Adprop");</v>
       </c>
-      <c r="L9" t="str">
+      <c r="J9" t="str">
         <f>CONCATENATE("[",C9,"] [",A9,"] ",E9,",")</f>
         <v>[Created] [datetime] NULL,</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -10207,26 +9559,19 @@
       <c r="G10" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" s="15" t="s">
+      <c r="H10" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="J10" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I10" s="1" t="str">
+        <f>CONCATENATE("collist[",F10,"] = new TableColDefEx(""",C10,""", typeof(",B10,"), """,H10,""",""",G10,""");")</f>
         <v>collist[8] = new TableColDefEx("Description", typeof(String), "description","Adprop");</v>
       </c>
-      <c r="K10" t="str">
-        <f t="shared" ref="K10:K12" si="4">CONCATENATE("row[",F10,"] = computer.",I10,";")</f>
-        <v>row[8] = computer.description;</v>
-      </c>
-      <c r="L10" t="str">
-        <f t="shared" ref="L10:L13" si="5">CONCATENATE("[",C10,"] [",A10,"](",D10,") ",E10,",")</f>
+      <c r="J10" t="str">
+        <f>CONCATENATE("[",C10,"] [",A10,"](",D10,") ",E10,",")</f>
         <v>[Description] [nvarchar](256) NULL,</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -10248,26 +9593,19 @@
       <c r="G11" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I11" s="15" t="s">
+      <c r="H11" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="J11" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I11" s="1" t="str">
+        <f>CONCATENATE("collist[",F11,"] = new TableColDefEx(""",C11,""", typeof(",B11,"), """,H11,""",""",G11,""");")</f>
         <v>collist[9] = new TableColDefEx("DisplayName", typeof(String), "displayname","Adprop");</v>
       </c>
-      <c r="K11" t="str">
-        <f t="shared" si="4"/>
-        <v>row[9] = computer.displayname;</v>
-      </c>
-      <c r="L11" t="str">
-        <f t="shared" si="5"/>
+      <c r="J11" t="str">
+        <f>CONCATENATE("[",C11,"] [",A11,"](",D11,") ",E11,",")</f>
         <v>[DisplayName] [nvarchar](128) NULL,</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -10289,26 +9627,19 @@
       <c r="G12" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I12" s="15" t="s">
+      <c r="H12" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="J12" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I12" s="1" t="str">
+        <f>CONCATENATE("collist[",F12,"] = new TableColDefEx(""",C12,""", typeof(",B12,"), """,H12,""",""",G12,""");")</f>
         <v>collist[10] = new TableColDefEx("DistinguishedName", typeof(String), "distinguishedname","Adprop");</v>
       </c>
-      <c r="K12" t="str">
-        <f t="shared" si="4"/>
-        <v>row[10] = computer.distinguishedname;</v>
-      </c>
-      <c r="L12" t="str">
-        <f t="shared" si="5"/>
+      <c r="J12" t="str">
+        <f>CONCATENATE("[",C12,"] [",A12,"](",D12,") ",E12,",")</f>
         <v>[DistinguishedName] [nvarchar](512) NULL,</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -10330,22 +9661,19 @@
       <c r="G13" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H13" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13" s="15" t="s">
+      <c r="H13" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="J13" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I13" s="1" t="str">
+        <f>CONCATENATE("collist[",F13,"] = new TableColDefEx(""",C13,""", typeof(",B13,"), """,H13,""",""",G13,""");")</f>
         <v>collist[11] = new TableColDefEx("DNSHostName", typeof(String), "dnshostname","Adprop");</v>
       </c>
-      <c r="L13" t="str">
-        <f t="shared" si="5"/>
+      <c r="J13" t="str">
+        <f>CONCATENATE("[",C13,"] [",A13,"](",D13,") ",E13,",")</f>
         <v>[DNSHostName] [nvarchar](128) NULL,</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -10364,26 +9692,19 @@
       <c r="G14" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I14" s="17" t="s">
+      <c r="H14" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="J14" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I14" s="1" t="str">
+        <f>CONCATENATE("collist[",F14,"] = new TableColDefEx(""",C14,""", typeof(",B14,"), """,H14,""",""",G14,""");")</f>
         <v>collist[12] = new TableColDefEx("DoesNotRequirePreAuth", typeof(Boolean), "DONT_REQ_PREAUTH","UAC");</v>
       </c>
-      <c r="K14" t="str">
-        <f>CONCATENATE("row[",F14,"] = ((uac &amp; ",I14,") != 0) ? true : false;")</f>
-        <v>row[12] = ((uac &amp; DONT_REQ_PREAUTH) != 0) ? true : false;</v>
-      </c>
-      <c r="L14" t="str">
+      <c r="J14" t="str">
         <f>CONCATENATE("[",C14,"] [",A14,"] ",E14,",")</f>
         <v>[DoesNotRequirePreAuth] [bit] NULL,</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -10402,26 +9723,19 @@
       <c r="G15" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H15" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I15" s="17" t="s">
+      <c r="H15" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="J15" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I15" s="1" t="str">
+        <f>CONCATENATE("collist[",F15,"] = new TableColDefEx(""",C15,""", typeof(",B15,"), """,H15,""",""",G15,""");")</f>
         <v>collist[13] = new TableColDefEx("Enabled", typeof(Boolean), "ACCOUNTDISABLE","UAC");</v>
       </c>
-      <c r="K15" t="str">
-        <f>CONCATENATE("row[",F15,"] = computer.",I15,";")</f>
-        <v>row[13] = computer.ACCOUNTDISABLE;</v>
-      </c>
-      <c r="L15" t="str">
+      <c r="J15" t="str">
         <f>CONCATENATE("[",C15,"] [",A15,"] ",E15,",")</f>
         <v>[Enabled] [bit] NULL,</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -10440,26 +9754,19 @@
       <c r="G16" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="H16" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I16" s="16" t="s">
+      <c r="H16" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="J16" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I16" s="1" t="str">
+        <f>CONCATENATE("collist[",F16,"] = new TableColDefEx(""",C16,""", typeof(",B16,"), """,H16,""",""",G16,""");")</f>
         <v>collist[14] = new TableColDefEx("LastBadPasswordAttempt", typeof(DateTime), "badpasswordtime","filetime");</v>
       </c>
-      <c r="K16" t="str">
-        <f t="shared" ref="K16:K17" si="6">CONCATENATE("if(computer.",I16," !=null) row[",F16,"] = computer.",I16,";")</f>
-        <v>if(computer.badpasswordtime !=null) row[14] = computer.badpasswordtime;</v>
-      </c>
-      <c r="L16" t="str">
-        <f t="shared" ref="L16:L23" si="7">CONCATENATE("[",C16,"] [",A16,"] ",E16,",")</f>
+      <c r="J16" t="str">
+        <f>CONCATENATE("[",C16,"] [",A16,"] ",E16,",")</f>
         <v>[LastBadPasswordAttempt] [datetime] NULL,</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -10478,26 +9785,19 @@
       <c r="G17" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="H17" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I17" s="16" t="s">
+      <c r="H17" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="J17" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I17" s="1" t="str">
+        <f>CONCATENATE("collist[",F17,"] = new TableColDefEx(""",C17,""", typeof(",B17,"), """,H17,""",""",G17,""");")</f>
         <v>collist[15] = new TableColDefEx("LastLogonDate", typeof(DateTime), "lastlogontimestamp/lastlogon","filetime");</v>
       </c>
-      <c r="K17" t="str">
-        <f t="shared" si="6"/>
-        <v>if(computer.lastlogontimestamp/lastlogon !=null) row[15] = computer.lastlogontimestamp/lastlogon;</v>
-      </c>
-      <c r="L17" t="str">
-        <f t="shared" si="7"/>
+      <c r="J17" t="str">
+        <f>CONCATENATE("[",C17,"] [",A17,"] ",E17,",")</f>
         <v>[LastLogonDate] [datetime] NULL,</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -10519,22 +9819,19 @@
       <c r="G18" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H18" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I18" s="15" t="s">
+      <c r="H18" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="J18" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I18" s="1" t="str">
+        <f>CONCATENATE("collist[",F18,"] = new TableColDefEx(""",C18,""", typeof(",B18,"), """,H18,""",""",G18,""");")</f>
         <v>collist[16] = new TableColDefEx("Location", typeof(String), "location","Adprop");</v>
       </c>
-      <c r="L18" t="str">
-        <f t="shared" ref="L18" si="8">CONCATENATE("[",C18,"] [",A18,"](",D18,") ",E18,",")</f>
+      <c r="J18" t="str">
+        <f>CONCATENATE("[",C18,"] [",A18,"](",D18,") ",E18,",")</f>
         <v>[Location] [nvarchar](128) NULL,</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -10553,26 +9850,19 @@
       <c r="G19" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I19" s="17" t="s">
+      <c r="H19" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="J19" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I19" s="1" t="str">
+        <f>CONCATENATE("collist[",F19,"] = new TableColDefEx(""",C19,""", typeof(",B19,"), """,H19,""",""",G19,""");")</f>
         <v>collist[17] = new TableColDefEx("LockedOut", typeof(Boolean), "LOCKOUT","UAC");</v>
       </c>
-      <c r="K19" t="str">
-        <f>CONCATENATE("row[",F19,"] = computer.",I19,"();")</f>
-        <v>row[17] = computer.LOCKOUT();</v>
-      </c>
-      <c r="L19" t="str">
-        <f t="shared" si="7"/>
+      <c r="J19" t="str">
+        <f>CONCATENATE("[",C19,"] [",A19,"] ",E19,",")</f>
         <v>[LockedOut] [bit] NULL,</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -10591,22 +9881,19 @@
       <c r="G20" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H20" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="H20" t="s">
         <v>147</v>
       </c>
-      <c r="J20" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I20" s="1" t="str">
+        <f>CONCATENATE("collist[",F20,"] = new TableColDefEx(""",C20,""", typeof(",B20,"), """,H20,""",""",G20,""");")</f>
         <v>collist[18] = new TableColDefEx("logonCount", typeof(Int32), "logoncount","Adprop");</v>
       </c>
-      <c r="L20" t="str">
-        <f t="shared" si="7"/>
+      <c r="J20" t="str">
+        <f>CONCATENATE("[",C20,"] [",A20,"] ",E20,",")</f>
         <v>[logonCount] [int] NULL,</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -10628,22 +9915,19 @@
       <c r="G21" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H21" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I21" s="15" t="s">
+      <c r="H21" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="J21" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I21" s="1" t="str">
+        <f>CONCATENATE("collist[",F21,"] = new TableColDefEx(""",C21,""", typeof(",B21,"), """,H21,""",""",G21,""");")</f>
         <v>collist[19] = new TableColDefEx("ManagedBy", typeof(String), "managedby","Adprop");</v>
       </c>
-      <c r="L21" t="str">
-        <f t="shared" ref="L21" si="9">CONCATENATE("[",C21,"] [",A21,"](",D21,") ",E21,",")</f>
+      <c r="J21" t="str">
+        <f>CONCATENATE("[",C21,"] [",A21,"](",D21,") ",E21,",")</f>
         <v>[ManagedBy] [nvarchar](256) NULL,</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -10662,22 +9946,19 @@
       <c r="G22" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H22" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I22" s="15" t="s">
+      <c r="H22" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="J22" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I22" s="1" t="str">
+        <f>CONCATENATE("collist[",F22,"] = new TableColDefEx(""",C22,""", typeof(",B22,"), """,H22,""",""",G22,""");")</f>
         <v>collist[20] = new TableColDefEx("Modified", typeof(DateTime), "whenChanged","Adprop");</v>
       </c>
-      <c r="L22" t="str">
-        <f t="shared" si="7"/>
+      <c r="J22" t="str">
+        <f>CONCATENATE("[",C22,"] [",A22,"] ",E22,",")</f>
         <v>[Modified] [datetime] NULL,</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -10696,22 +9977,19 @@
       <c r="G23" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H23" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I23" s="17" t="s">
+      <c r="H23" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="J23" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I23" s="1" t="str">
+        <f>CONCATENATE("collist[",F23,"] = new TableColDefEx(""",C23,""", typeof(",B23,"), """,H23,""",""",G23,""");")</f>
         <v>collist[21] = new TableColDefEx("MNSLogonAccount", typeof(Boolean), "MNS_LOGON_ACCOUNT","UAC");</v>
       </c>
-      <c r="L23" t="str">
-        <f t="shared" si="7"/>
+      <c r="J23" t="str">
+        <f>CONCATENATE("[",C23,"] [",A23,"] ",E23,",")</f>
         <v>[MNSLogonAccount] [bit] NULL,</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -10733,26 +10011,19 @@
       <c r="G24" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H24" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I24" s="15" t="s">
+      <c r="H24" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="J24" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I24" s="1" t="str">
+        <f>CONCATENATE("collist[",F24,"] = new TableColDefEx(""",C24,""", typeof(",B24,"), """,H24,""",""",G24,""");")</f>
         <v>collist[22] = new TableColDefEx("Name", typeof(String), "name","Adprop");</v>
       </c>
-      <c r="K24" t="str">
-        <f>CONCATENATE("row[",F24,"] = computer.",I24,";")</f>
-        <v>row[22] = computer.name;</v>
-      </c>
-      <c r="L24" t="str">
-        <f t="shared" ref="L24:L30" si="10">CONCATENATE("[",C24,"] [",A24,"](",D24,") ",E24,",")</f>
+      <c r="J24" t="str">
+        <f>CONCATENATE("[",C24,"] [",A24,"](",D24,") ",E24,",")</f>
         <v>[Name] [nvarchar](256) NULL,</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -10774,22 +10045,19 @@
       <c r="G25" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H25" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I25" s="15" t="s">
+      <c r="H25" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="J25" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I25" s="1" t="str">
+        <f>CONCATENATE("collist[",F25,"] = new TableColDefEx(""",C25,""", typeof(",B25,"), """,H25,""",""",G25,""");")</f>
         <v>collist[23] = new TableColDefEx("ObjectCategory", typeof(String), "objectcategory","Adprop");</v>
       </c>
-      <c r="L25" t="str">
-        <f t="shared" si="10"/>
+      <c r="J25" t="str">
+        <f>CONCATENATE("[",C25,"] [",A25,"](",D25,") ",E25,",")</f>
         <v>[ObjectCategory] [nvarchar](128) NULL,</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -10811,26 +10079,19 @@
       <c r="G26" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="H26" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I26" s="15" t="s">
+      <c r="H26" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="J26" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I26" s="1" t="str">
+        <f>CONCATENATE("collist[",F26,"] = new TableColDefEx(""",C26,""", typeof(",B26,"), """,H26,""",""",G26,""");")</f>
         <v>collist[24] = new TableColDefEx("ObjectClass", typeof(String), "SchemaClassName","ObjClass");</v>
       </c>
-      <c r="K26" t="str">
-        <f t="shared" ref="K26:K27" si="11">CONCATENATE("row[",F26,"] = computer.",I26,";")</f>
-        <v>row[24] = computer.SchemaClassName;</v>
-      </c>
-      <c r="L26" t="str">
-        <f t="shared" si="10"/>
+      <c r="J26" t="str">
+        <f>CONCATENATE("[",C26,"] [",A26,"](",D26,") ",E26,",")</f>
         <v>[ObjectClass] [nvarchar](64) NULL,</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -10849,26 +10110,19 @@
       <c r="G27" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H27" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I27" s="15" t="s">
+      <c r="H27" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I27" s="1" t="str">
+        <f>CONCATENATE("collist[",F27,"] = new TableColDefEx(""",C27,""", typeof(",B27,"), """,H27,""",""",G27,""");")</f>
         <v>collist[25] = new TableColDefEx("ObjectGUID", typeof(Guid), "Guid","ObjGuid");</v>
       </c>
-      <c r="K27" t="str">
-        <f t="shared" si="11"/>
-        <v>row[25] = computer.Guid;</v>
-      </c>
-      <c r="L27" t="str">
+      <c r="J27" t="str">
         <f>CONCATENATE("[",C27,"] [",A27,"] ",E27,",")</f>
         <v>[ObjectGUID] [uniqueidentifier] NOT NULL,</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -10890,22 +10144,19 @@
       <c r="G28" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H28" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="H28" t="s">
         <v>148</v>
       </c>
-      <c r="J28" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I28" s="1" t="str">
+        <f>CONCATENATE("collist[",F28,"] = new TableColDefEx(""",C28,""", typeof(",B28,"), """,H28,""",""",G28,""");")</f>
         <v>collist[26] = new TableColDefEx("OperatingSystem", typeof(String), "operatingsystem","Adprop");</v>
       </c>
-      <c r="L28" t="str">
-        <f t="shared" si="10"/>
+      <c r="J28" t="str">
+        <f>CONCATENATE("[",C28,"] [",A28,"](",D28,") ",E28,",")</f>
         <v>[OperatingSystem] [nvarchar](64) NULL,</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -10927,22 +10178,19 @@
       <c r="G29" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H29" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="H29" t="s">
         <v>151</v>
       </c>
-      <c r="J29" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I29" s="1" t="str">
+        <f>CONCATENATE("collist[",F29,"] = new TableColDefEx(""",C29,""", typeof(",B29,"), """,H29,""",""",G29,""");")</f>
         <v>collist[27] = new TableColDefEx("OperatingSystemServicePack", typeof(String), "operatingsystemservicepack","Adprop");</v>
       </c>
-      <c r="L29" t="str">
-        <f t="shared" si="10"/>
+      <c r="J29" t="str">
+        <f>CONCATENATE("[",C29,"] [",A29,"](",D29,") ",E29,",")</f>
         <v>[OperatingSystemServicePack] [nvarchar](32) NULL,</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -10964,22 +10212,19 @@
       <c r="G30" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H30" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I30" t="s">
+      <c r="H30" t="s">
         <v>154</v>
       </c>
-      <c r="J30" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I30" s="1" t="str">
+        <f>CONCATENATE("collist[",F30,"] = new TableColDefEx(""",C30,""", typeof(",B30,"), """,H30,""",""",G30,""");")</f>
         <v>collist[28] = new TableColDefEx("OperatingSystemVersion", typeof(String), "operatingsystemversion","Adprop");</v>
       </c>
-      <c r="L30" t="str">
-        <f t="shared" si="10"/>
+      <c r="J30" t="str">
+        <f>CONCATENATE("[",C30,"] [",A30,"](",D30,") ",E30,",")</f>
         <v>[OperatingSystemVersion] [nvarchar](16) NULL,</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -10998,26 +10243,19 @@
       <c r="G31" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H31" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I31" s="17" t="s">
+      <c r="H31" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="J31" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I31" s="1" t="str">
+        <f>CONCATENATE("collist[",F31,"] = new TableColDefEx(""",C31,""", typeof(",B31,"), """,H31,""",""",G31,""");")</f>
         <v>collist[29] = new TableColDefEx("PasswordExpired", typeof(Boolean), "PASSWORD_EXPIRED","UAC");</v>
       </c>
-      <c r="K31" t="str">
-        <f>CONCATENATE("row[",F31,"] = ((uac &amp; ",I31,") != 0) ? true : false;")</f>
-        <v>row[29] = ((uac &amp; PASSWORD_EXPIRED) != 0) ? true : false;</v>
-      </c>
-      <c r="L31" t="str">
-        <f t="shared" ref="L31:L34" si="12">CONCATENATE("[",C31,"] [",A31,"] ",E31,",")</f>
+      <c r="J31" t="str">
+        <f>CONCATENATE("[",C31,"] [",A31,"] ",E31,",")</f>
         <v>[PasswordExpired] [bit] NULL,</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -11036,26 +10274,19 @@
       <c r="G32" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="H32" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I32" s="16" t="s">
+      <c r="H32" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="J32" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I32" s="1" t="str">
+        <f>CONCATENATE("collist[",F32,"] = new TableColDefEx(""",C32,""", typeof(",B32,"), """,H32,""",""",G32,""");")</f>
         <v>collist[30] = new TableColDefEx("PasswordLastSet", typeof(DateTime), "pwdlastset","filetime");</v>
       </c>
-      <c r="K32" t="str">
-        <f>CONCATENATE("if(computer.",I32," !=null) row[",F32,"] = computer.",I32,";")</f>
-        <v>if(computer.pwdlastset !=null) row[30] = computer.pwdlastset;</v>
-      </c>
-      <c r="L32" t="str">
-        <f t="shared" si="12"/>
+      <c r="J32" t="str">
+        <f>CONCATENATE("[",C32,"] [",A32,"] ",E32,",")</f>
         <v>[PasswordLastSet] [datetime] NULL,</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -11074,26 +10305,19 @@
       <c r="G33" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H33" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I33" s="17" t="s">
+      <c r="H33" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="J33" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I33" s="1" t="str">
+        <f>CONCATENATE("collist[",F33,"] = new TableColDefEx(""",C33,""", typeof(",B33,"), """,H33,""",""",G33,""");")</f>
         <v>collist[31] = new TableColDefEx("PasswordNeverExpires", typeof(Boolean), "DONT_EXPIRE_PASSWD","UAC");</v>
       </c>
-      <c r="K33" t="str">
-        <f t="shared" ref="K33:K34" si="13">CONCATENATE("row[",F33,"] = computer.",I33,";")</f>
-        <v>row[31] = computer.DONT_EXPIRE_PASSWD;</v>
-      </c>
-      <c r="L33" t="str">
-        <f t="shared" si="12"/>
+      <c r="J33" t="str">
+        <f>CONCATENATE("[",C33,"] [",A33,"] ",E33,",")</f>
         <v>[PasswordNeverExpires] [bit] NULL,</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -11112,26 +10336,19 @@
       <c r="G34" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H34" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I34" s="17" t="s">
+      <c r="H34" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="J34" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I34" s="1" t="str">
+        <f>CONCATENATE("collist[",F34,"] = new TableColDefEx(""",C34,""", typeof(",B34,"), """,H34,""",""",G34,""");")</f>
         <v>collist[32] = new TableColDefEx("PasswordNotRequired", typeof(Boolean), "PASSWD_NOTREQD","UAC");</v>
       </c>
-      <c r="K34" t="str">
-        <f t="shared" si="13"/>
-        <v>row[32] = computer.PASSWD_NOTREQD;</v>
-      </c>
-      <c r="L34" t="str">
-        <f t="shared" si="12"/>
+      <c r="J34" t="str">
+        <f>CONCATENATE("[",C34,"] [",A34,"] ",E34,",")</f>
         <v>[PasswordNotRequired] [bit] NULL,</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -11153,22 +10370,19 @@
       <c r="G35" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H35" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I35" s="15" t="s">
+      <c r="H35" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="J35" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I35" s="1" t="str">
+        <f>CONCATENATE("collist[",F35,"] = new TableColDefEx(""",C35,""", typeof(",B35,"), """,H35,""",""",G35,""");")</f>
         <v>collist[33] = new TableColDefEx("PrimaryGroupID", typeof(Int32), "primarygroupid","Adprop");</v>
       </c>
-      <c r="L35" t="str">
+      <c r="J35" t="str">
         <f>CONCATENATE("[",C35,"] [",A35,"] ",E35,",")</f>
         <v>[PrimaryGroupID] [int] NULL,</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -11190,26 +10404,19 @@
       <c r="G36" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H36" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I36" s="15" t="s">
+      <c r="H36" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="J36" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I36" s="1" t="str">
+        <f>CONCATENATE("collist[",F36,"] = new TableColDefEx(""",C36,""", typeof(",B36,"), """,H36,""",""",G36,""");")</f>
         <v>collist[34] = new TableColDefEx("SamAccountName", typeof(String), "samaccountname","Adprop");</v>
       </c>
-      <c r="K36" t="str">
-        <f t="shared" ref="K36:K38" si="14">CONCATENATE("row[",F36,"] = computer.",I36,";")</f>
-        <v>row[34] = computer.samaccountname;</v>
-      </c>
-      <c r="L36" t="str">
-        <f t="shared" ref="L36:L37" si="15">CONCATENATE("[",C36,"] [",A36,"](",D36,") ",E36,",")</f>
+      <c r="J36" t="str">
+        <f>CONCATENATE("[",C36,"] [",A36,"](",D36,") ",E36,",")</f>
         <v>[SamAccountName] [nvarchar](128) NULL,</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -11231,26 +10438,19 @@
       <c r="G37" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H37" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I37" s="15" t="s">
+      <c r="H37" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="J37" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I37" s="1" t="str">
+        <f>CONCATENATE("collist[",F37,"] = new TableColDefEx(""",C37,""", typeof(",B37,"), """,H37,""",""",G37,""");")</f>
         <v>collist[35] = new TableColDefEx("SID", typeof(String), "objectsid","SID");</v>
       </c>
-      <c r="K37" t="str">
-        <f t="shared" si="14"/>
-        <v>row[35] = computer.objectsid;</v>
-      </c>
-      <c r="L37" t="str">
-        <f t="shared" si="15"/>
+      <c r="J37" t="str">
+        <f>CONCATENATE("[",C37,"] [",A37,"](",D37,") ",E37,",")</f>
         <v>[SID] [nvarchar](128) NOT NULL,</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -11269,26 +10469,19 @@
       <c r="G38" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H38" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I38" s="17" t="s">
+      <c r="H38" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="J38" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I38" s="1" t="str">
+        <f>CONCATENATE("collist[",F38,"] = new TableColDefEx(""",C38,""", typeof(",B38,"), """,H38,""",""",G38,""");")</f>
         <v>collist[36] = new TableColDefEx("SmartcardLogonRequired", typeof(Boolean), "SMARTCARD_REQUIRED","UAC");</v>
       </c>
-      <c r="K38" t="str">
-        <f t="shared" si="14"/>
-        <v>row[36] = computer.SMARTCARD_REQUIRED;</v>
-      </c>
-      <c r="L38" t="str">
+      <c r="J38" t="str">
         <f>CONCATENATE("[",C38,"] [",A38,"] ",E38,",")</f>
         <v>[SmartcardLogonRequired] [bit] NULL,</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -11307,26 +10500,19 @@
       <c r="G39" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H39" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I39" s="17" t="s">
+      <c r="H39" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="J39" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I39" s="1" t="str">
+        <f>CONCATENATE("collist[",F39,"] = new TableColDefEx(""",C39,""", typeof(",B39,"), """,H39,""",""",G39,""");")</f>
         <v>collist[37] = new TableColDefEx("TrustedForDelegation", typeof(Boolean), "TRUSTED_FOR_DELEGATION","UAC");</v>
       </c>
-      <c r="K39" t="str">
-        <f t="shared" ref="K39:K41" si="16">CONCATENATE("row[",F39,"] = ((uac &amp; ",I39,") != 0) ? true : false;")</f>
-        <v>row[37] = ((uac &amp; TRUSTED_FOR_DELEGATION) != 0) ? true : false;</v>
-      </c>
-      <c r="L39" t="str">
-        <f t="shared" ref="L39:L43" si="17">CONCATENATE("[",C39,"] [",A39,"] ",E39,",")</f>
+      <c r="J39" t="str">
+        <f t="shared" ref="J39:J43" si="0">CONCATENATE("[",C39,"] [",A39,"] ",E39,",")</f>
         <v>[TrustedForDelegation] [bit] NULL,</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -11345,26 +10531,19 @@
       <c r="G40" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H40" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I40" s="17" t="s">
+      <c r="H40" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="J40" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I40" s="1" t="str">
+        <f>CONCATENATE("collist[",F40,"] = new TableColDefEx(""",C40,""", typeof(",B40,"), """,H40,""",""",G40,""");")</f>
         <v>collist[38] = new TableColDefEx("TrustedToAuthForDelegation", typeof(Boolean), "TRUSTED_TO_AUTH_FOR_DELEGATION","UAC");</v>
       </c>
-      <c r="K40" t="str">
-        <f t="shared" si="16"/>
-        <v>row[38] = ((uac &amp; TRUSTED_TO_AUTH_FOR_DELEGATION) != 0) ? true : false;</v>
-      </c>
-      <c r="L40" t="str">
-        <f t="shared" si="17"/>
+      <c r="J40" t="str">
+        <f t="shared" si="0"/>
         <v>[TrustedToAuthForDelegation] [bit] NULL,</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -11383,26 +10562,19 @@
       <c r="G41" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H41" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I41" s="17" t="s">
+      <c r="H41" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="J41" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I41" s="1" t="str">
+        <f>CONCATENATE("collist[",F41,"] = new TableColDefEx(""",C41,""", typeof(",B41,"), """,H41,""",""",G41,""");")</f>
         <v>collist[39] = new TableColDefEx("UseDESKeyOnly", typeof(Boolean), "USE_DES_KEY_ONLY","UAC");</v>
       </c>
-      <c r="K41" t="str">
-        <f t="shared" si="16"/>
-        <v>row[39] = ((uac &amp; USE_DES_KEY_ONLY) != 0) ? true : false;</v>
-      </c>
-      <c r="L41" t="str">
-        <f t="shared" si="17"/>
+      <c r="J41" t="str">
+        <f t="shared" si="0"/>
         <v>[UseDESKeyOnly] [bit] NULL,</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -11421,24 +10593,579 @@
       <c r="G42" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H42" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I42" s="15" t="s">
+      <c r="H42" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="J42" s="1" t="str">
-        <f t="shared" si="0"/>
+      <c r="I42" s="1" t="str">
+        <f>CONCATENATE("collist[",F42,"] = new TableColDefEx(""",C42,""", typeof(",B42,"), """,H42,""",""",G42,""");")</f>
         <v>collist[40] = new TableColDefEx("userAccountControl", typeof(Int32), "useraccountcontrol","Adprop");</v>
       </c>
-      <c r="L42" t="str">
+      <c r="J42" t="str">
         <f>CONCATENATE("[",C42,"] [",A42,"] ",E42,",")</f>
         <v>[userAccountControl] [int] NULL,</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L43"/>
+  <autoFilter ref="A1:J43"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1"/>
+    <col min="9" max="9" width="88.140625" customWidth="1"/>
+    <col min="10" max="10" width="44.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>CONCATENATE("collist[",F2,"] = new TableColDefEx(""",C2,""", typeof(",B2,"), """,H2,""",""",G2,""");")</f>
+        <v>collist[0] = new TableColDefEx("Created", typeof(DateTime), "whenCreated","Adprop");</v>
+      </c>
+      <c r="J2" t="str">
+        <f>CONCATENATE("[",C2,"] [",A2,"] ",E2,",")</f>
+        <v>[Created] [datetime] NULL,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>256</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f t="shared" ref="I3:I16" si="0">CONCATENATE("collist[",F3,"] = new TableColDefEx(""",C3,""", typeof(",B3,"), """,H3,""",""",G3,""");")</f>
+        <v>collist[1] = new TableColDefEx("Description", typeof(String), "description","Adprop");</v>
+      </c>
+      <c r="J3" t="str">
+        <f>CONCATENATE("[",C3,"] [",A3,"](",D3,") ",E3,",")</f>
+        <v>[Description] [nvarchar](256) NULL,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>128</v>
+      </c>
+      <c r="E4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[2] = new TableColDefEx("DisplayName", typeof(String), "displayname","Adprop");</v>
+      </c>
+      <c r="J4" t="str">
+        <f>CONCATENATE("[",C4,"] [",A4,"](",D4,") ",E4,",")</f>
+        <v>[DisplayName] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>512</v>
+      </c>
+      <c r="E5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="6">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[3] = new TableColDefEx("DistinguishedName", typeof(String), "distinguishedname","Adprop");</v>
+      </c>
+      <c r="J5" t="str">
+        <f>CONCATENATE("[",C5,"] [",A5,"](",D5,") ",E5,",")</f>
+        <v>[DistinguishedName] [nvarchar](512) NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>256</v>
+      </c>
+      <c r="E6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[4] = new TableColDefEx("EmailAddress", typeof(String), "mail","Adprop");</v>
+      </c>
+      <c r="J6" t="str">
+        <f>CONCATENATE("[",C6,"] [",A6,"](",D6,") ",E6,",")</f>
+        <v>[EmailAddress] [nvarchar](256) NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="6">
+        <v>5</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[5] = new TableColDefEx("GroupCategory", typeof(String), "grouptype","GrpCat");</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" ref="J7:J8" si="1">CONCATENATE("[",C7,"] [",A7,"](",D7,") ",E7,",")</f>
+        <v>[GroupCategory] [nvarchar](32) NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="6">
+        <v>6</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[6] = new TableColDefEx("GroupScope", typeof(String), "grouptype","GrpScope");</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="1"/>
+        <v>[GroupScope] [nvarchar](32) NULL,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9">
+        <v>256</v>
+      </c>
+      <c r="E9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="6">
+        <v>7</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[7] = new TableColDefEx("ManagedBy", typeof(String), "managedby","Adprop");</v>
+      </c>
+      <c r="J9" t="str">
+        <f>CONCATENATE("[",C9,"] [",A9,"](",D9,") ",E9,",")</f>
+        <v>[ManagedBy] [nvarchar](256) NULL,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="6">
+        <v>8</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[8] = new TableColDefEx("Modified", typeof(DateTime), "whenChanged","Adprop");</v>
+      </c>
+      <c r="J10" t="str">
+        <f>CONCATENATE("[",C10,"] [",A10,"] ",E10,",")</f>
+        <v>[Modified] [datetime] NULL,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11">
+        <v>256</v>
+      </c>
+      <c r="E11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="6">
+        <v>9</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[9] = new TableColDefEx("Name", typeof(String), "name","Adprop");</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" ref="J11:J13" si="2">CONCATENATE("[",C11,"] [",A11,"](",D11,") ",E11,",")</f>
+        <v>[Name] [nvarchar](256) NULL,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12">
+        <v>128</v>
+      </c>
+      <c r="E12" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="6">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[10] = new TableColDefEx("ObjectCategory", typeof(String), "objectcategory","Adprop");</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="2"/>
+        <v>[ObjectCategory] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13">
+        <v>64</v>
+      </c>
+      <c r="E13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="6">
+        <v>11</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[11] = new TableColDefEx("ObjectClass", typeof(String), "SchemaClassName","ObjClass");</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="2"/>
+        <v>[ObjectClass] [nvarchar](64) NULL,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" s="6">
+        <v>12</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[12] = new TableColDefEx("ObjectGUID", typeof(Guid), "Guid","ObjGuid");</v>
+      </c>
+      <c r="J14" t="str">
+        <f>CONCATENATE("[",C14,"] [",A14,"] ",E14,",")</f>
+        <v>[ObjectGUID] [uniqueidentifier] NOT NULL,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15">
+        <v>128</v>
+      </c>
+      <c r="E15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="6">
+        <v>13</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[13] = new TableColDefEx("SamAccountName", typeof(String), "samaccountname","Adprop");</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" ref="J15:J16" si="3">CONCATENATE("[",C15,"] [",A15,"](",D15,") ",E15,",")</f>
+        <v>[SamAccountName] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16">
+        <v>128</v>
+      </c>
+      <c r="E16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F16" s="6">
+        <v>14</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[14] = new TableColDefEx("SID", typeof(String), "objectsid","SID");</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="3"/>
+        <v>[SID] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J16"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added get contacts to clr_GetADobjects
</commit_message>
<xml_diff>
--- a/GetADobjects/AD_DW_Users table map to .net V4.xlsx
+++ b/GetADobjects/AD_DW_Users table map to .net V4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" tabRatio="625" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" tabRatio="625" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,16 @@
     <sheet name="Computers" sheetId="4" r:id="rId3"/>
     <sheet name="Groups" sheetId="5" r:id="rId4"/>
     <sheet name="Users (2)" sheetId="9" r:id="rId5"/>
-    <sheet name="Computers (2)" sheetId="8" r:id="rId6"/>
-    <sheet name="Groups (2)" sheetId="7" r:id="rId7"/>
+    <sheet name="Contacts (2)" sheetId="11" r:id="rId6"/>
+    <sheet name="Computers (2)" sheetId="8" r:id="rId7"/>
+    <sheet name="Groups (2)" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Computers!$A$1:$L$38</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Computers (2)'!$A$1:$J$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Computers (2)'!$A$1:$J$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Contacts (2)'!$A$1:$J$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Groups!$A$1:$L$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Groups (2)'!$A$1:$J$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Groups (2)'!$A$1:$J$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Users!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Users (2)'!$A$1:$J$68</definedName>
   </definedNames>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="204">
   <si>
     <t>max_length</t>
   </si>
@@ -7012,8 +7014,2232 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="6"/>
+    <col min="8" max="8" width="34.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="120" customWidth="1"/>
+    <col min="10" max="10" width="40.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>CONCATENATE("collist[",F2,"] = new TableColDefEx(""",C2,""", typeof(",B2,"), """,H2,""",""",G2,""");")</f>
+        <v>collist[0] = new TableColDefEx("AccountExpirationDate", typeof(DateTime), "accountexpires","filetime");</v>
+      </c>
+      <c r="J2" t="str">
+        <f>CONCATENATE("[",C2,"] [",A2,"] ",E2,",")</f>
+        <v>[AccountExpirationDate] [datetime] NULL,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f t="shared" ref="I3:I66" si="0">CONCATENATE("collist[",F3,"] = new TableColDefEx(""",C3,""", typeof(",B3,"), """,H3,""",""",G3,""");")</f>
+        <v>collist[1] = new TableColDefEx("AccountLockoutTime", typeof(DateTime), "lockouttime","filetime");</v>
+      </c>
+      <c r="J3" t="str">
+        <f>CONCATENATE("[",C3,"] [",A3,"] ",E3,",")</f>
+        <v>[AccountLockoutTime] [datetime] NULL,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[2] = new TableColDefEx("AccountNotDelegated", typeof(Boolean), "NOT_DELEGATED","UAC");</v>
+      </c>
+      <c r="J4" t="str">
+        <f>CONCATENATE("[",C4,"] [",A4,"] ",E4,",")</f>
+        <v>[AccountNotDelegated] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="6">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[3] = new TableColDefEx("AllowReversiblePasswordEncryption", typeof(Boolean), "ENCRYPTED_TEXT_PWD_ALLOWED","UAC");</v>
+      </c>
+      <c r="J5" t="str">
+        <f>CONCATENATE("[",C5,"] [",A5,"] ",E5,",")</f>
+        <v>[AllowReversiblePasswordEncryption] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[4] = new TableColDefEx("BadLogonCount", typeof(Int32), "badpwdcount","Adprop");</v>
+      </c>
+      <c r="J6" t="str">
+        <f>CONCATENATE("[",C6,"] [",A6,"] ",E6,",")</f>
+        <v>[BadLogonCount] [int] NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="6">
+        <v>5</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[5] = new TableColDefEx("CannotChangePassword", typeof(Boolean), "PASSWD_CANT_CHANGE","UAC");</v>
+      </c>
+      <c r="J7" t="str">
+        <f>CONCATENATE("[",C7,"] [",A7,"] ",E7,",")</f>
+        <v>[CannotChangePassword] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>128</v>
+      </c>
+      <c r="E8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="6">
+        <v>6</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[6] = new TableColDefEx("City", typeof(String), "l","Adprop");</v>
+      </c>
+      <c r="J8" t="str">
+        <f>CONCATENATE("[",C8,"] [",A8,"](",D8,") ",E8,",")</f>
+        <v>[City] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>256</v>
+      </c>
+      <c r="E9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="6">
+        <v>7</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[7] = new TableColDefEx("CN", typeof(String), "cn","Adprop");</v>
+      </c>
+      <c r="J9" t="str">
+        <f>CONCATENATE("[",C9,"] [",A9,"](",D9,") ",E9,",")</f>
+        <v>[CN] [nvarchar](256) NULL,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>128</v>
+      </c>
+      <c r="E10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="6">
+        <v>8</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[8] = new TableColDefEx("Company", typeof(String), "company","Adprop");</v>
+      </c>
+      <c r="J10" t="str">
+        <f>CONCATENATE("[",C10,"] [",A10,"](",D10,") ",E10,",")</f>
+        <v>[Company] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>128</v>
+      </c>
+      <c r="E11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="6">
+        <v>9</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[9] = new TableColDefEx("Country", typeof(String), "co","Adprop");</v>
+      </c>
+      <c r="J11" t="str">
+        <f>CONCATENATE("[",C11,"] [",A11,"](",D11,") ",E11,",")</f>
+        <v>[Country] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="6">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[10] = new TableColDefEx("Created", typeof(DateTime), "whencreated","Adprop");</v>
+      </c>
+      <c r="J12" t="str">
+        <f>CONCATENATE("[",C12,"] [",A12,"] ",E12,",")</f>
+        <v>[Created] [datetime] NULL,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>128</v>
+      </c>
+      <c r="E13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="6">
+        <v>11</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[11] = new TableColDefEx("Department", typeof(String), "department","Adprop");</v>
+      </c>
+      <c r="J13" t="str">
+        <f>CONCATENATE("[",C13,"] [",A13,"](",D13,") ",E13,",")</f>
+        <v>[Department] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14">
+        <v>256</v>
+      </c>
+      <c r="E14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="6">
+        <v>12</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[12] = new TableColDefEx("Description", typeof(String), "description","Adprop");</v>
+      </c>
+      <c r="J14" t="str">
+        <f>CONCATENATE("[",C14,"] [",A14,"](",D14,") ",E14,",")</f>
+        <v>[Description] [nvarchar](256) NULL,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>128</v>
+      </c>
+      <c r="E15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="6">
+        <v>13</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[13] = new TableColDefEx("DisplayName", typeof(String), "displayname","Adprop");</v>
+      </c>
+      <c r="J15" t="str">
+        <f>CONCATENATE("[",C15,"] [",A15,"](",D15,") ",E15,",")</f>
+        <v>[DisplayName] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>512</v>
+      </c>
+      <c r="E16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F16" s="6">
+        <v>14</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[14] = new TableColDefEx("DistinguishedName", typeof(String), "distinguishedname","Adprop");</v>
+      </c>
+      <c r="J16" t="str">
+        <f>CONCATENATE("[",C16,"] [",A16,"](",D16,") ",E16,",")</f>
+        <v>[DistinguishedName] [nvarchar](512) NULL,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17">
+        <v>128</v>
+      </c>
+      <c r="E17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="6">
+        <v>15</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[15] = new TableColDefEx("Division", typeof(String), "division","Adprop");</v>
+      </c>
+      <c r="J17" t="str">
+        <f>CONCATENATE("[",C17,"] [",A17,"](",D17,") ",E17,",")</f>
+        <v>[Division] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="6">
+        <v>16</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[16] = new TableColDefEx("DoesNotRequirePreAuth", typeof(Boolean), "DONT_REQ_PREAUTH","UAC");</v>
+      </c>
+      <c r="J18" t="str">
+        <f>CONCATENATE("[",C18,"] [",A18,"] ",E18,",")</f>
+        <v>[DoesNotRequirePreAuth] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19">
+        <v>256</v>
+      </c>
+      <c r="E19" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="6">
+        <v>17</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[17] = new TableColDefEx("EmailAddress", typeof(String), "mail","Adprop");</v>
+      </c>
+      <c r="J19" t="str">
+        <f>CONCATENATE("[",C19,"] [",A19,"](",D19,") ",E19,",")</f>
+        <v>[EmailAddress] [nvarchar](256) NULL,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="6">
+        <v>18</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[18] = new TableColDefEx("EmployeeID", typeof(String), "employeeid","Adprop");</v>
+      </c>
+      <c r="J20" t="str">
+        <f>CONCATENATE("[",C20,"] [",A20,"](",D20,") ",E20,",")</f>
+        <v>[EmployeeID] [nvarchar](64) NULL,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21">
+        <v>64</v>
+      </c>
+      <c r="E21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="6">
+        <v>19</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[19] = new TableColDefEx("EmployeeNumber", typeof(String), "employeenumber","Adprop");</v>
+      </c>
+      <c r="J21" t="str">
+        <f>CONCATENATE("[",C21,"] [",A21,"](",D21,") ",E21,",")</f>
+        <v>[EmployeeNumber] [nvarchar](64) NULL,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" s="6">
+        <v>20</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[20] = new TableColDefEx("Enabled", typeof(Boolean), "ACCOUNTDISABLE","UAC");</v>
+      </c>
+      <c r="J22" t="str">
+        <f>CONCATENATE("[",C22,"] [",A22,"] ",E22,",")</f>
+        <v>[Enabled] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23">
+        <v>128</v>
+      </c>
+      <c r="E23" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="6">
+        <v>21</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[21] = new TableColDefEx("Fax", typeof(String), "facsimileTelephoneNumber","Adprop");</v>
+      </c>
+      <c r="J23" t="str">
+        <f>CONCATENATE("[",C23,"] [",A23,"](",D23,") ",E23,",")</f>
+        <v>[Fax] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24">
+        <v>128</v>
+      </c>
+      <c r="E24" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="6">
+        <v>22</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[22] = new TableColDefEx("GivenName", typeof(String), "givenname","Adprop");</v>
+      </c>
+      <c r="J24" t="str">
+        <f>CONCATENATE("[",C24,"] [",A24,"](",D24,") ",E24,",")</f>
+        <v>[GivenName] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25">
+        <v>128</v>
+      </c>
+      <c r="E25" t="s">
+        <v>115</v>
+      </c>
+      <c r="F25" s="6">
+        <v>23</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[23] = new TableColDefEx("HomeDirectory", typeof(String), "homedirectory","Adprop");</v>
+      </c>
+      <c r="J25" t="str">
+        <f>CONCATENATE("[",C25,"] [",A25,"](",D25,") ",E25,",")</f>
+        <v>[HomeDirectory] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="6">
+        <v>24</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[24] = new TableColDefEx("HomedirRequired", typeof(Boolean), "HOMEDIR_REQUIRED","UAC");</v>
+      </c>
+      <c r="J26" t="str">
+        <f>CONCATENATE("[",C26,"] [",A26,"] ",E26,",")</f>
+        <v>[HomedirRequired] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27">
+        <v>64</v>
+      </c>
+      <c r="E27" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="6">
+        <v>25</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[25] = new TableColDefEx("HomeDrive", typeof(String), "homedrive","Adprop");</v>
+      </c>
+      <c r="J27" t="str">
+        <f>CONCATENATE("[",C27,"] [",A27,"](",D27,") ",E27,",")</f>
+        <v>[HomeDrive] [nvarchar](64) NULL,</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28">
+        <v>128</v>
+      </c>
+      <c r="E28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="6">
+        <v>26</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[26] = new TableColDefEx("HomePage", typeof(String), "wwwhomepage","Adprop");</v>
+      </c>
+      <c r="J28" t="str">
+        <f>CONCATENATE("[",C28,"] [",A28,"](",D28,") ",E28,",")</f>
+        <v>[HomePage] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29">
+        <v>32</v>
+      </c>
+      <c r="E29" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="6">
+        <v>27</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[27] = new TableColDefEx("HomePhone", typeof(String), "homephone","Adprop");</v>
+      </c>
+      <c r="J29" t="str">
+        <f>CONCATENATE("[",C29,"] [",A29,"](",D29,") ",E29,",")</f>
+        <v>[HomePhone] [nvarchar](32) NULL,</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30">
+        <v>32</v>
+      </c>
+      <c r="E30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="6">
+        <v>28</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H30" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[28] = new TableColDefEx("Initials", typeof(String), "initials","Adprop");</v>
+      </c>
+      <c r="J30" t="str">
+        <f>CONCATENATE("[",C30,"] [",A30,"](",D30,") ",E30,",")</f>
+        <v>[Initials] [nvarchar](32) NULL,</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="6">
+        <v>29</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[29] = new TableColDefEx("LastBadPasswordAttempt", typeof(DateTime), "badpasswordtime","filetime");</v>
+      </c>
+      <c r="J31" t="str">
+        <f>CONCATENATE("[",C31,"] [",A31,"] ",E31,",")</f>
+        <v>[LastBadPasswordAttempt] [datetime] NULL,</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="6">
+        <v>30</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="I32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[30] = new TableColDefEx("LastLogonDate", typeof(DateTime), "lastlogon","filetime");</v>
+      </c>
+      <c r="J32" t="str">
+        <f>CONCATENATE("[",C32,"] [",A32,"] ",E32,",")</f>
+        <v>[LastLogonDate] [datetime] NULL,</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" s="6">
+        <v>31</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="I33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[31] = new TableColDefEx("LockedOut", typeof(Boolean), "LOCKOUT","UAC");</v>
+      </c>
+      <c r="J33" t="str">
+        <f>CONCATENATE("[",C33,"] [",A33,"] ",E33,",")</f>
+        <v>[LockedOut] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E34" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="6">
+        <v>32</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[32] = new TableColDefEx("LogonCount", typeof(Int32), "logoncount","Adprop");</v>
+      </c>
+      <c r="J34" t="str">
+        <f>CONCATENATE("[",C34,"] [",A34,"] ",E34,",")</f>
+        <v>[LogonCount] [int] NULL,</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35">
+        <v>128</v>
+      </c>
+      <c r="E35" t="s">
+        <v>115</v>
+      </c>
+      <c r="F35" s="6">
+        <v>33</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="I35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[33] = new TableColDefEx("LogonWorkstations", typeof(String), "userworkstations","Adprop");</v>
+      </c>
+      <c r="J35" t="str">
+        <f>CONCATENATE("[",C35,"] [",A35,"](",D35,") ",E35,",")</f>
+        <v>[LogonWorkstations] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36">
+        <v>256</v>
+      </c>
+      <c r="E36" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" s="6">
+        <v>34</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H36" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="I36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[34] = new TableColDefEx("Manager", typeof(String), "manager","Adprop");</v>
+      </c>
+      <c r="J36" t="str">
+        <f>CONCATENATE("[",C36,"] [",A36,"](",D36,") ",E36,",")</f>
+        <v>[Manager] [nvarchar](256) NULL,</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" s="6">
+        <v>35</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[35] = new TableColDefEx("MNSLogonAccount", typeof(Boolean), "MNS_LOGON_ACCOUNT","UAC");</v>
+      </c>
+      <c r="J37" t="str">
+        <f>CONCATENATE("[",C37,"] [",A37,"] ",E37,",")</f>
+        <v>[MNSLogonAccount] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38">
+        <v>32</v>
+      </c>
+      <c r="E38" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="6">
+        <v>36</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[36] = new TableColDefEx("MobilePhone", typeof(String), "mobile","Adprop");</v>
+      </c>
+      <c r="J38" t="str">
+        <f>CONCATENATE("[",C38,"] [",A38,"](",D38,") ",E38,",")</f>
+        <v>[MobilePhone] [nvarchar](32) NULL,</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="6">
+        <v>37</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="I39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[37] = new TableColDefEx("Modified", typeof(DateTime), "whenchanged","Adprop");</v>
+      </c>
+      <c r="J39" t="str">
+        <f>CONCATENATE("[",C39,"] [",A39,"] ",E39,",")</f>
+        <v>[Modified] [datetime] NULL,</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40">
+        <v>256</v>
+      </c>
+      <c r="E40" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="6">
+        <v>38</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="I40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[38] = new TableColDefEx("Name", typeof(String), "name","Adprop");</v>
+      </c>
+      <c r="J40" t="str">
+        <f>CONCATENATE("[",C40,"] [",A40,"](",D40,") ",E40,",")</f>
+        <v>[Name] [nvarchar](256) NULL,</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41">
+        <v>128</v>
+      </c>
+      <c r="E41" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="6">
+        <v>39</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="I41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[39] = new TableColDefEx("ObjectCategory", typeof(String), "objectcategory","Adprop");</v>
+      </c>
+      <c r="J41" t="str">
+        <f>CONCATENATE("[",C41,"] [",A41,"](",D41,") ",E41,",")</f>
+        <v>[ObjectCategory] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42">
+        <v>64</v>
+      </c>
+      <c r="E42" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="6">
+        <v>40</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="I42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[40] = new TableColDefEx("ObjectClass", typeof(String), "SchemaClassName","ObjClass");</v>
+      </c>
+      <c r="J42" t="str">
+        <f>CONCATENATE("[",C42,"] [",A42,"](",D42,") ",E42,",")</f>
+        <v>[ObjectClass] [nvarchar](64) NULL,</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" t="s">
+        <v>116</v>
+      </c>
+      <c r="F43" s="6">
+        <v>41</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="I43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[41] = new TableColDefEx("ObjectGUID", typeof(Guid), "Guid","ObjGuid");</v>
+      </c>
+      <c r="J43" t="str">
+        <f>CONCATENATE("[",C43,"] [",A43,"] ",E43,",")</f>
+        <v>[ObjectGUID] [uniqueidentifier] NOT NULL,</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44">
+        <v>128</v>
+      </c>
+      <c r="E44" t="s">
+        <v>115</v>
+      </c>
+      <c r="F44" s="6">
+        <v>42</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="I44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[42] = new TableColDefEx("Office", typeof(String), "physicalDeliveryOfficeName","Adprop");</v>
+      </c>
+      <c r="J44" t="str">
+        <f>CONCATENATE("[",C44,"] [",A44,"](",D44,") ",E44,",")</f>
+        <v>[Office] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45">
+        <v>32</v>
+      </c>
+      <c r="E45" t="s">
+        <v>115</v>
+      </c>
+      <c r="F45" s="6">
+        <v>43</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="I45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[43] = new TableColDefEx("OfficePhone", typeof(String), "telephonenumber","Adprop");</v>
+      </c>
+      <c r="J45" t="str">
+        <f>CONCATENATE("[",C45,"] [",A45,"](",D45,") ",E45,",")</f>
+        <v>[OfficePhone] [nvarchar](32) NULL,</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46">
+        <v>32</v>
+      </c>
+      <c r="E46" t="s">
+        <v>115</v>
+      </c>
+      <c r="F46" s="6">
+        <v>44</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="I46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[44] = new TableColDefEx("Pager", typeof(String), "pager","Adprop");</v>
+      </c>
+      <c r="J46" t="str">
+        <f>CONCATENATE("[",C46,"] [",A46,"](",D46,") ",E46,",")</f>
+        <v>[Pager] [nvarchar](32) NULL,</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47" s="6">
+        <v>45</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H47" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[45] = new TableColDefEx("PasswordExpired", typeof(Boolean), "PASSWORD_EXPIRED","UAC");</v>
+      </c>
+      <c r="J47" t="str">
+        <f>CONCATENATE("[",C47,"] [",A47,"] ",E47,",")</f>
+        <v>[PasswordExpired] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" t="s">
+        <v>115</v>
+      </c>
+      <c r="F48" s="6">
+        <v>46</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H48" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="I48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[46] = new TableColDefEx("PasswordLastSet", typeof(DateTime), "pwdlastset","filetime");</v>
+      </c>
+      <c r="J48" t="str">
+        <f>CONCATENATE("[",C48,"] [",A48,"] ",E48,",")</f>
+        <v>[PasswordLastSet] [datetime] NULL,</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" t="s">
+        <v>115</v>
+      </c>
+      <c r="F49" s="6">
+        <v>47</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="I49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[47] = new TableColDefEx("PasswordNeverExpires", typeof(Boolean), "DONT_EXPIRE_PASSWD","UAC");</v>
+      </c>
+      <c r="J49" t="str">
+        <f>CONCATENATE("[",C49,"] [",A49,"] ",E49,",")</f>
+        <v>[PasswordNeverExpires] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" t="s">
+        <v>53</v>
+      </c>
+      <c r="E50" t="s">
+        <v>115</v>
+      </c>
+      <c r="F50" s="6">
+        <v>48</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H50" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="I50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[48] = new TableColDefEx("PasswordNotRequired", typeof(Boolean), "PASSWD_NOTREQD","UAC");</v>
+      </c>
+      <c r="J50" t="str">
+        <f>CONCATENATE("[",C50,"] [",A50,"] ",E50,",")</f>
+        <v>[PasswordNotRequired] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51">
+        <v>32</v>
+      </c>
+      <c r="E51" t="s">
+        <v>115</v>
+      </c>
+      <c r="F51" s="6">
+        <v>49</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H51" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="I51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[49] = new TableColDefEx("POBox", typeof(String), "postofficebox","Adprop");</v>
+      </c>
+      <c r="J51" t="str">
+        <f>CONCATENATE("[",C51,"] [",A51,"](",D51,") ",E51,",")</f>
+        <v>[POBox] [nvarchar](32) NULL,</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52">
+        <v>32</v>
+      </c>
+      <c r="E52" t="s">
+        <v>115</v>
+      </c>
+      <c r="F52" s="6">
+        <v>50</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H52" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="I52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[50] = new TableColDefEx("PostalCode", typeof(String), "postalcode","Adprop");</v>
+      </c>
+      <c r="J52" t="str">
+        <f>CONCATENATE("[",C52,"] [",A52,"](",D52,") ",E52,",")</f>
+        <v>[PostalCode] [nvarchar](32) NULL,</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53">
+        <v>128</v>
+      </c>
+      <c r="E53" t="s">
+        <v>115</v>
+      </c>
+      <c r="F53" s="6">
+        <v>51</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[51] = new TableColDefEx("PrimaryGroupID", typeof(Int32), "primarygroupid","Adprop");</v>
+      </c>
+      <c r="J53" t="str">
+        <f>CONCATENATE("[",C53,"] [",A53,"] ",E53,",")</f>
+        <v>[PrimaryGroupID] [int] NULL,</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" t="s">
+        <v>83</v>
+      </c>
+      <c r="C54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54">
+        <v>128</v>
+      </c>
+      <c r="E54" t="s">
+        <v>115</v>
+      </c>
+      <c r="F54" s="6">
+        <v>52</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="I54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[52] = new TableColDefEx("ProfilePath", typeof(String), "profilepath","Adprop");</v>
+      </c>
+      <c r="J54" t="str">
+        <f>CONCATENATE("[",C54,"] [",A54,"](",D54,") ",E54,",")</f>
+        <v>[ProfilePath] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" t="s">
+        <v>83</v>
+      </c>
+      <c r="C55" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55">
+        <v>128</v>
+      </c>
+      <c r="E55" t="s">
+        <v>115</v>
+      </c>
+      <c r="F55" s="6">
+        <v>53</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="I55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[53] = new TableColDefEx("SamAccountName", typeof(String), "samaccountname","Adprop");</v>
+      </c>
+      <c r="J55" t="str">
+        <f>CONCATENATE("[",C55,"] [",A55,"](",D55,") ",E55,",")</f>
+        <v>[SamAccountName] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" t="s">
+        <v>83</v>
+      </c>
+      <c r="C56" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56">
+        <v>256</v>
+      </c>
+      <c r="E56" t="s">
+        <v>115</v>
+      </c>
+      <c r="F56" s="6">
+        <v>54</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H56" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="I56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[54] = new TableColDefEx("ScriptPath", typeof(String), "scriptpath","Adprop");</v>
+      </c>
+      <c r="J56" t="str">
+        <f>CONCATENATE("[",C56,"] [",A56,"](",D56,") ",E56,",")</f>
+        <v>[ScriptPath] [nvarchar](256) NULL,</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57">
+        <v>128</v>
+      </c>
+      <c r="E57" t="s">
+        <v>116</v>
+      </c>
+      <c r="F57" s="6">
+        <v>55</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="I57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[55] = new TableColDefEx("SID", typeof(String), "objectsid","SID");</v>
+      </c>
+      <c r="J57" t="str">
+        <f>CONCATENATE("[",C57,"] [",A57,"](",D57,") ",E57,",")</f>
+        <v>[SID] [nvarchar](128) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58" t="s">
+        <v>60</v>
+      </c>
+      <c r="E58" t="s">
+        <v>115</v>
+      </c>
+      <c r="F58" s="6">
+        <v>56</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="I58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[56] = new TableColDefEx("SmartcardLogonRequired", typeof(Boolean), "SMARTCARD_REQUIRED","UAC");</v>
+      </c>
+      <c r="J58" t="str">
+        <f>CONCATENATE("[",C58,"] [",A58,"] ",E58,",")</f>
+        <v>[SmartcardLogonRequired] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59">
+        <v>64</v>
+      </c>
+      <c r="E59" t="s">
+        <v>115</v>
+      </c>
+      <c r="F59" s="6">
+        <v>57</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="I59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[57] = new TableColDefEx("State", typeof(String), "st","Adprop");</v>
+      </c>
+      <c r="J59" t="str">
+        <f>CONCATENATE("[",C59,"] [",A59,"](",D59,") ",E59,",")</f>
+        <v>[State] [nvarchar](64) NULL,</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" t="s">
+        <v>83</v>
+      </c>
+      <c r="C60" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60">
+        <v>160</v>
+      </c>
+      <c r="E60" t="s">
+        <v>115</v>
+      </c>
+      <c r="F60" s="6">
+        <v>58</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="I60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[58] = new TableColDefEx("StreetAddress", typeof(String), "streetaddress","Adprop");</v>
+      </c>
+      <c r="J60" t="str">
+        <f>CONCATENATE("[",C60,"] [",A60,"](",D60,") ",E60,",")</f>
+        <v>[StreetAddress] [nvarchar](160) NULL,</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" t="s">
+        <v>83</v>
+      </c>
+      <c r="C61" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61">
+        <v>256</v>
+      </c>
+      <c r="E61" t="s">
+        <v>115</v>
+      </c>
+      <c r="F61" s="6">
+        <v>59</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="I61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[59] = new TableColDefEx("Surname", typeof(String), "sn","Adprop");</v>
+      </c>
+      <c r="J61" t="str">
+        <f>CONCATENATE("[",C61,"] [",A61,"](",D61,") ",E61,",")</f>
+        <v>[Surname] [nvarchar](256) NULL,</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" t="s">
+        <v>83</v>
+      </c>
+      <c r="C62" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62">
+        <v>128</v>
+      </c>
+      <c r="E62" t="s">
+        <v>115</v>
+      </c>
+      <c r="F62" s="6">
+        <v>60</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H62" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="I62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[60] = new TableColDefEx("Title", typeof(String), "title","Adprop");</v>
+      </c>
+      <c r="J62" t="str">
+        <f>CONCATENATE("[",C62,"] [",A62,"](",D62,") ",E62,",")</f>
+        <v>[Title] [nvarchar](128) NULL,</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E63" t="s">
+        <v>115</v>
+      </c>
+      <c r="F63" s="6">
+        <v>61</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H63" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="I63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[61] = new TableColDefEx("TrustedForDelegation", typeof(Boolean), "TRUSTED_FOR_DELEGATION","UAC");</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" ref="J63:J67" si="1">CONCATENATE("[",C63,"] [",A63,"] ",E63,",")</f>
+        <v>[TrustedForDelegation] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>80</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E64" t="s">
+        <v>115</v>
+      </c>
+      <c r="F64" s="6">
+        <v>62</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H64" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="I64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[62] = new TableColDefEx("TrustedToAuthForDelegation", typeof(Boolean), "TRUSTED_TO_AUTH_FOR_DELEGATION","UAC");</v>
+      </c>
+      <c r="J64" t="str">
+        <f t="shared" si="1"/>
+        <v>[TrustedToAuthForDelegation] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E65" t="s">
+        <v>115</v>
+      </c>
+      <c r="F65" s="6">
+        <v>63</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H65" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I65" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[63] = new TableColDefEx("UseDESKeyOnly", typeof(Boolean), "USE_DES_KEY_ONLY","UAC");</v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" si="1"/>
+        <v>[UseDESKeyOnly] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66" t="s">
+        <v>83</v>
+      </c>
+      <c r="C66" t="s">
+        <v>68</v>
+      </c>
+      <c r="D66">
+        <v>256</v>
+      </c>
+      <c r="E66" t="s">
+        <v>115</v>
+      </c>
+      <c r="F66" s="6">
+        <v>64</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H66" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="I66" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>collist[64] = new TableColDefEx("UserPrincipalName", typeof(String), "userprincipalname","Adprop");</v>
+      </c>
+      <c r="J66" t="str">
+        <f>CONCATENATE("[",C66,"] [",A66,"](",D66,") ",E66,",")</f>
+        <v>[UserPrincipalName] [nvarchar](256) NULL,</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" t="s">
+        <v>99</v>
+      </c>
+      <c r="E67" t="s">
+        <v>115</v>
+      </c>
+      <c r="F67" s="6">
+        <v>65</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H67" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="I67" s="1" t="str">
+        <f t="shared" ref="I67" si="2">CONCATENATE("collist[",F67,"] = new TableColDefEx(""",C67,""", typeof(",B67,"), """,H67,""",""",G67,""");")</f>
+        <v>collist[65] = new TableColDefEx("userAccountControl", typeof(Int32), "useraccountcontrol","Adprop");</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" si="1"/>
+        <v>[userAccountControl] [int] NULL,</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J68"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7063,13 +9289,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+        <v>83</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>128</v>
       </c>
       <c r="E2" t="s">
         <v>115</v>
@@ -7078,29 +9307,32 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>145</v>
+        <v>174</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>96</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>CONCATENATE("collist[",F2,"] = new TableColDefEx(""",C2,""", typeof(",B2,"), """,H2,""",""",G2,""");")</f>
-        <v>collist[0] = new TableColDefEx("AccountExpirationDate", typeof(DateTime), "accountexpires","filetime");</v>
+        <f t="shared" ref="I2:I35" si="0">CONCATENATE("collist[",F2,"] = new TableColDefEx(""",C2,""", typeof(",B2,"), """,H2,""",""",G2,""");")</f>
+        <v>collist[0] = new TableColDefEx("City", typeof(String), "l","Adprop");</v>
       </c>
       <c r="J2" t="str">
-        <f>CONCATENATE("[",C2,"] [",A2,"] ",E2,",")</f>
-        <v>[AccountExpirationDate] [datetime] NULL,</v>
+        <f>CONCATENATE("[",C2,"] [",A2,"](",D2,") ",E2,",")</f>
+        <v>[City] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>256</v>
       </c>
       <c r="E3" t="s">
         <v>115</v>
@@ -7109,29 +9341,32 @@
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>169</v>
+        <v>174</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>152</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I66" si="0">CONCATENATE("collist[",F3,"] = new TableColDefEx(""",C3,""", typeof(",B3,"), """,H3,""",""",G3,""");")</f>
-        <v>collist[1] = new TableColDefEx("AccountLockoutTime", typeof(DateTime), "lockouttime","filetime");</v>
+        <f t="shared" si="0"/>
+        <v>collist[1] = new TableColDefEx("CN", typeof(String), "cn","Adprop");</v>
       </c>
       <c r="J3" t="str">
-        <f>CONCATENATE("[",C3,"] [",A3,"] ",E3,",")</f>
-        <v>[AccountLockoutTime] [datetime] NULL,</v>
+        <f>CONCATENATE("[",C3,"] [",A3,"](",D3,") ",E3,",")</f>
+        <v>[CN] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>6</v>
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>128</v>
       </c>
       <c r="E4" t="s">
         <v>115</v>
@@ -7140,29 +9375,32 @@
         <v>2</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>105</v>
+        <v>174</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>181</v>
       </c>
       <c r="I4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[2] = new TableColDefEx("AccountNotDelegated", typeof(Boolean), "NOT_DELEGATED","UAC");</v>
+        <v>collist[2] = new TableColDefEx("Company", typeof(String), "company","Adprop");</v>
       </c>
       <c r="J4" t="str">
-        <f>CONCATENATE("[",C4,"] [",A4,"] ",E4,",")</f>
-        <v>[AccountNotDelegated] [bit] NULL,</v>
+        <f>CONCATENATE("[",C4,"] [",A4,"](",D4,") ",E4,",")</f>
+        <v>[Company] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
+        <v>83</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>128</v>
       </c>
       <c r="E5" t="s">
         <v>115</v>
@@ -7171,29 +9409,29 @@
         <v>3</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>168</v>
+        <v>174</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>89</v>
       </c>
       <c r="I5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[3] = new TableColDefEx("AllowReversiblePasswordEncryption", typeof(Boolean), "ENCRYPTED_TEXT_PWD_ALLOWED","UAC");</v>
+        <v>collist[3] = new TableColDefEx("Country", typeof(String), "co","Adprop");</v>
       </c>
       <c r="J5" t="str">
-        <f>CONCATENATE("[",C5,"] [",A5,"] ",E5,",")</f>
-        <v>[AllowReversiblePasswordEncryption] [bit] NULL,</v>
+        <f>CONCATENATE("[",C5,"] [",A5,"](",D5,") ",E5,",")</f>
+        <v>[Country] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
+        <v>81</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="E6" t="s">
         <v>115</v>
@@ -7205,26 +9443,29 @@
         <v>174</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
       <c r="I6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[4] = new TableColDefEx("BadLogonCount", typeof(Int32), "badpwdcount","Adprop");</v>
+        <v>collist[4] = new TableColDefEx("Created", typeof(DateTime), "whencreated","Adprop");</v>
       </c>
       <c r="J6" t="str">
         <f>CONCATENATE("[",C6,"] [",A6,"] ",E6,",")</f>
-        <v>[BadLogonCount] [int] NULL,</v>
+        <v>[Created] [datetime] NULL,</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>128</v>
       </c>
       <c r="E7" t="s">
         <v>115</v>
@@ -7233,18 +9474,18 @@
         <v>5</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>164</v>
+        <v>174</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>186</v>
       </c>
       <c r="I7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[5] = new TableColDefEx("CannotChangePassword", typeof(Boolean), "PASSWD_CANT_CHANGE","UAC");</v>
+        <v>collist[5] = new TableColDefEx("Department", typeof(String), "department","Adprop");</v>
       </c>
       <c r="J7" t="str">
-        <f>CONCATENATE("[",C7,"] [",A7,"] ",E7,",")</f>
-        <v>[CannotChangePassword] [bit] NULL,</v>
+        <f>CONCATENATE("[",C7,"] [",A7,"](",D7,") ",E7,",")</f>
+        <v>[Department] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -7254,11 +9495,11 @@
       <c r="B8" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>12</v>
+      <c r="C8" t="s">
+        <v>18</v>
       </c>
       <c r="D8">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="E8" t="s">
         <v>115</v>
@@ -7270,15 +9511,15 @@
         <v>174</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="I8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[6] = new TableColDefEx("City", typeof(String), "l","Adprop");</v>
+        <v>collist[6] = new TableColDefEx("Description", typeof(String), "description","Adprop");</v>
       </c>
       <c r="J8" t="str">
         <f>CONCATENATE("[",C8,"] [",A8,"](",D8,") ",E8,",")</f>
-        <v>[City] [nvarchar](128) NULL,</v>
+        <v>[Description] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -7289,10 +9530,10 @@
         <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D9">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="E9" t="s">
         <v>115</v>
@@ -7304,15 +9545,15 @@
         <v>174</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="I9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[7] = new TableColDefEx("CN", typeof(String), "cn","Adprop");</v>
+        <v>collist[7] = new TableColDefEx("DisplayName", typeof(String), "displayname","Adprop");</v>
       </c>
       <c r="J9" t="str">
         <f>CONCATENATE("[",C9,"] [",A9,"](",D9,") ",E9,",")</f>
-        <v>[CN] [nvarchar](256) NULL,</v>
+        <v>[DisplayName] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -7323,10 +9564,10 @@
         <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="E10" t="s">
         <v>115</v>
@@ -7338,15 +9579,15 @@
         <v>174</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>181</v>
+        <v>140</v>
       </c>
       <c r="I10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[8] = new TableColDefEx("Company", typeof(String), "company","Adprop");</v>
+        <v>collist[8] = new TableColDefEx("DistinguishedName", typeof(String), "distinguishedname","Adprop");</v>
       </c>
       <c r="J10" t="str">
         <f>CONCATENATE("[",C10,"] [",A10,"](",D10,") ",E10,",")</f>
-        <v>[Company] [nvarchar](128) NULL,</v>
+        <v>[DistinguishedName] [nvarchar](512) NULL,</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -7356,8 +9597,8 @@
       <c r="B11" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>15</v>
+      <c r="C11" t="s">
+        <v>21</v>
       </c>
       <c r="D11">
         <v>128</v>
@@ -7372,26 +9613,29 @@
         <v>174</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>89</v>
+        <v>188</v>
       </c>
       <c r="I11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[9] = new TableColDefEx("Country", typeof(String), "co","Adprop");</v>
+        <v>collist[9] = new TableColDefEx("Division", typeof(String), "division","Adprop");</v>
       </c>
       <c r="J11" t="str">
         <f>CONCATENATE("[",C11,"] [",A11,"](",D11,") ",E11,",")</f>
-        <v>[Country] [nvarchar](128) NULL,</v>
+        <v>[Division] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>16</v>
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>256</v>
       </c>
       <c r="E12" t="s">
         <v>115</v>
@@ -7403,15 +9647,15 @@
         <v>174</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>184</v>
+        <v>123</v>
       </c>
       <c r="I12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[10] = new TableColDefEx("Created", typeof(DateTime), "whencreated","Adprop");</v>
+        <v>collist[10] = new TableColDefEx("EmailAddress", typeof(String), "mail","Adprop");</v>
       </c>
       <c r="J12" t="str">
-        <f>CONCATENATE("[",C12,"] [",A12,"] ",E12,",")</f>
-        <v>[Created] [datetime] NULL,</v>
+        <f>CONCATENATE("[",C12,"] [",A12,"](",D12,") ",E12,",")</f>
+        <v>[EmailAddress] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -7422,10 +9666,10 @@
         <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D13">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
         <v>115</v>
@@ -7437,15 +9681,15 @@
         <v>174</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[11] = new TableColDefEx("Department", typeof(String), "department","Adprop");</v>
+        <v>collist[11] = new TableColDefEx("EmployeeID", typeof(String), "employeeid","Adprop");</v>
       </c>
       <c r="J13" t="str">
         <f>CONCATENATE("[",C13,"] [",A13,"](",D13,") ",E13,",")</f>
-        <v>[Department] [nvarchar](128) NULL,</v>
+        <v>[EmployeeID] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -7456,10 +9700,10 @@
         <v>83</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D14">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
         <v>115</v>
@@ -7471,15 +9715,15 @@
         <v>174</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="I14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[12] = new TableColDefEx("Description", typeof(String), "description","Adprop");</v>
+        <v>collist[12] = new TableColDefEx("EmployeeNumber", typeof(String), "employeenumber","Adprop");</v>
       </c>
       <c r="J14" t="str">
         <f>CONCATENATE("[",C14,"] [",A14,"](",D14,") ",E14,",")</f>
-        <v>[Description] [nvarchar](256) NULL,</v>
+        <v>[EmployeeNumber] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -7489,8 +9733,8 @@
       <c r="B15" t="s">
         <v>83</v>
       </c>
-      <c r="C15" t="s">
-        <v>19</v>
+      <c r="C15" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D15">
         <v>128</v>
@@ -7505,15 +9749,15 @@
         <v>174</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="I15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[13] = new TableColDefEx("DisplayName", typeof(String), "displayname","Adprop");</v>
+        <v>collist[13] = new TableColDefEx("Fax", typeof(String), "facsimileTelephoneNumber","Adprop");</v>
       </c>
       <c r="J15" t="str">
         <f>CONCATENATE("[",C15,"] [",A15,"](",D15,") ",E15,",")</f>
-        <v>[DisplayName] [nvarchar](128) NULL,</v>
+        <v>[Fax] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -7524,10 +9768,10 @@
         <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D16">
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="E16" t="s">
         <v>115</v>
@@ -7539,15 +9783,15 @@
         <v>174</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>140</v>
+        <v>177</v>
       </c>
       <c r="I16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[14] = new TableColDefEx("DistinguishedName", typeof(String), "distinguishedname","Adprop");</v>
+        <v>collist[14] = new TableColDefEx("GivenName", typeof(String), "givenname","Adprop");</v>
       </c>
       <c r="J16" t="str">
         <f>CONCATENATE("[",C16,"] [",A16,"](",D16,") ",E16,",")</f>
-        <v>[DistinguishedName] [nvarchar](512) NULL,</v>
+        <v>[GivenName] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -7557,8 +9801,8 @@
       <c r="B17" t="s">
         <v>83</v>
       </c>
-      <c r="C17" t="s">
-        <v>21</v>
+      <c r="C17" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="D17">
         <v>128</v>
@@ -7573,26 +9817,29 @@
         <v>174</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[15] = new TableColDefEx("Division", typeof(String), "division","Adprop");</v>
+        <v>collist[15] = new TableColDefEx("HomePage", typeof(String), "wwwhomepage","Adprop");</v>
       </c>
       <c r="J17" t="str">
         <f>CONCATENATE("[",C17,"] [",A17,"](",D17,") ",E17,",")</f>
-        <v>[Division] [nvarchar](128) NULL,</v>
+        <v>[HomePage] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>22</v>
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <v>32</v>
       </c>
       <c r="E18" t="s">
         <v>115</v>
@@ -7601,18 +9848,18 @@
         <v>16</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>107</v>
+        <v>187</v>
       </c>
       <c r="I18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[16] = new TableColDefEx("DoesNotRequirePreAuth", typeof(Boolean), "DONT_REQ_PREAUTH","UAC");</v>
+        <v>collist[16] = new TableColDefEx("HomePhone", typeof(String), "homephone","Adprop");</v>
       </c>
       <c r="J18" t="str">
-        <f>CONCATENATE("[",C18,"] [",A18,"] ",E18,",")</f>
-        <v>[DoesNotRequirePreAuth] [bit] NULL,</v>
+        <f>CONCATENATE("[",C18,"] [",A18,"](",D18,") ",E18,",")</f>
+        <v>[HomePhone] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -7623,10 +9870,10 @@
         <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D19">
-        <v>256</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
         <v>115</v>
@@ -7638,15 +9885,15 @@
         <v>174</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>123</v>
+        <v>183</v>
       </c>
       <c r="I19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[17] = new TableColDefEx("EmailAddress", typeof(String), "mail","Adprop");</v>
+        <v>collist[17] = new TableColDefEx("Initials", typeof(String), "initials","Adprop");</v>
       </c>
       <c r="J19" t="str">
         <f>CONCATENATE("[",C19,"] [",A19,"](",D19,") ",E19,",")</f>
-        <v>[EmailAddress] [nvarchar](256) NULL,</v>
+        <v>[Initials] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -7657,10 +9904,10 @@
         <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D20">
-        <v>64</v>
+        <v>256</v>
       </c>
       <c r="E20" t="s">
         <v>115</v>
@@ -7672,15 +9919,15 @@
         <v>174</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="I20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[18] = new TableColDefEx("EmployeeID", typeof(String), "employeeid","Adprop");</v>
+        <v>collist[18] = new TableColDefEx("Manager", typeof(String), "manager","Adprop");</v>
       </c>
       <c r="J20" t="str">
         <f>CONCATENATE("[",C20,"] [",A20,"](",D20,") ",E20,",")</f>
-        <v>[EmployeeID] [nvarchar](64) NULL,</v>
+        <v>[Manager] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -7690,11 +9937,11 @@
       <c r="B21" t="s">
         <v>83</v>
       </c>
-      <c r="C21" t="s">
-        <v>25</v>
+      <c r="C21" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="D21">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E21" t="s">
         <v>115</v>
@@ -7706,26 +9953,26 @@
         <v>174</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>189</v>
+        <v>95</v>
       </c>
       <c r="I21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[19] = new TableColDefEx("EmployeeNumber", typeof(String), "employeenumber","Adprop");</v>
+        <v>collist[19] = new TableColDefEx("MobilePhone", typeof(String), "mobile","Adprop");</v>
       </c>
       <c r="J21" t="str">
         <f>CONCATENATE("[",C21,"] [",A21,"](",D21,") ",E21,",")</f>
-        <v>[EmployeeNumber] [nvarchar](64) NULL,</v>
+        <v>[MobilePhone] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" t="s">
-        <v>26</v>
+        <v>81</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="E22" t="s">
         <v>115</v>
@@ -7734,18 +9981,18 @@
         <v>20</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="I22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[20] = new TableColDefEx("Enabled", typeof(Boolean), "ACCOUNTDISABLE","UAC");</v>
+        <v>collist[20] = new TableColDefEx("Modified", typeof(DateTime), "whenchanged","Adprop");</v>
       </c>
       <c r="J22" t="str">
         <f>CONCATENATE("[",C22,"] [",A22,"] ",E22,",")</f>
-        <v>[Enabled] [bit] NULL,</v>
+        <v>[Modified] [datetime] NULL,</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -7755,11 +10002,11 @@
       <c r="B23" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>27</v>
+      <c r="C23" t="s">
+        <v>43</v>
       </c>
       <c r="D23">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="E23" t="s">
         <v>115</v>
@@ -7771,15 +10018,15 @@
         <v>174</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="I23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[21] = new TableColDefEx("Fax", typeof(String), "facsimileTelephoneNumber","Adprop");</v>
+        <v>collist[21] = new TableColDefEx("Name", typeof(String), "name","Adprop");</v>
       </c>
       <c r="J23" t="str">
         <f>CONCATENATE("[",C23,"] [",A23,"](",D23,") ",E23,",")</f>
-        <v>[Fax] [nvarchar](128) NULL,</v>
+        <v>[Name] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -7790,7 +10037,7 @@
         <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D24">
         <v>128</v>
@@ -7805,15 +10052,15 @@
         <v>174</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>177</v>
+        <v>139</v>
       </c>
       <c r="I24" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[22] = new TableColDefEx("GivenName", typeof(String), "givenname","Adprop");</v>
+        <v>collist[22] = new TableColDefEx("ObjectCategory", typeof(String), "objectcategory","Adprop");</v>
       </c>
       <c r="J24" t="str">
         <f>CONCATENATE("[",C24,"] [",A24,"](",D24,") ",E24,",")</f>
-        <v>[GivenName] [nvarchar](128) NULL,</v>
+        <v>[ObjectCategory] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -7823,11 +10070,11 @@
       <c r="B25" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>29</v>
+      <c r="C25" t="s">
+        <v>45</v>
       </c>
       <c r="D25">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
         <v>115</v>
@@ -7836,49 +10083,49 @@
         <v>23</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>190</v>
+        <v>144</v>
       </c>
       <c r="I25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[23] = new TableColDefEx("HomeDirectory", typeof(String), "homedirectory","Adprop");</v>
+        <v>collist[23] = new TableColDefEx("ObjectClass", typeof(String), "SchemaClassName","ObjClass");</v>
       </c>
       <c r="J25" t="str">
         <f>CONCATENATE("[",C25,"] [",A25,"](",D25,") ",E25,",")</f>
-        <v>[HomeDirectory] [nvarchar](128) NULL,</v>
+        <v>[ObjectClass] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>30</v>
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
       </c>
       <c r="E26" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F26" s="6">
         <v>24</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="I26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[24] = new TableColDefEx("HomedirRequired", typeof(Boolean), "HOMEDIR_REQUIRED","UAC");</v>
+        <v>collist[24] = new TableColDefEx("ObjectGUID", typeof(Guid), "Guid","ObjGuid");</v>
       </c>
       <c r="J26" t="str">
         <f>CONCATENATE("[",C26,"] [",A26,"] ",E26,",")</f>
-        <v>[HomedirRequired] [bit] NULL,</v>
+        <v>[ObjectGUID] [uniqueidentifier] NOT NULL,</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -7889,10 +10136,10 @@
         <v>83</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D27">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="E27" t="s">
         <v>115</v>
@@ -7904,15 +10151,15 @@
         <v>174</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>191</v>
+        <v>91</v>
       </c>
       <c r="I27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[25] = new TableColDefEx("HomeDrive", typeof(String), "homedrive","Adprop");</v>
+        <v>collist[25] = new TableColDefEx("Office", typeof(String), "physicalDeliveryOfficeName","Adprop");</v>
       </c>
       <c r="J27" t="str">
         <f>CONCATENATE("[",C27,"] [",A27,"](",D27,") ",E27,",")</f>
-        <v>[HomeDrive] [nvarchar](64) NULL,</v>
+        <v>[Office] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -7923,10 +10170,10 @@
         <v>83</v>
       </c>
       <c r="C28" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28">
         <v>32</v>
-      </c>
-      <c r="D28">
-        <v>128</v>
       </c>
       <c r="E28" t="s">
         <v>115</v>
@@ -7938,15 +10185,15 @@
         <v>174</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="I28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[26] = new TableColDefEx("HomePage", typeof(String), "wwwhomepage","Adprop");</v>
+        <v>collist[26] = new TableColDefEx("OfficePhone", typeof(String), "telephonenumber","Adprop");</v>
       </c>
       <c r="J28" t="str">
         <f>CONCATENATE("[",C28,"] [",A28,"](",D28,") ",E28,",")</f>
-        <v>[HomePage] [nvarchar](128) NULL,</v>
+        <v>[OfficePhone] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -7957,7 +10204,7 @@
         <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="D29">
         <v>32</v>
@@ -7972,15 +10219,15 @@
         <v>174</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="I29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[27] = new TableColDefEx("HomePhone", typeof(String), "homephone","Adprop");</v>
+        <v>collist[27] = new TableColDefEx("Pager", typeof(String), "pager","Adprop");</v>
       </c>
       <c r="J29" t="str">
         <f>CONCATENATE("[",C29,"] [",A29,"](",D29,") ",E29,",")</f>
-        <v>[HomePhone] [nvarchar](32) NULL,</v>
+        <v>[Pager] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -7990,8 +10237,8 @@
       <c r="B30" t="s">
         <v>83</v>
       </c>
-      <c r="C30" t="s">
-        <v>34</v>
+      <c r="C30" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="D30">
         <v>32</v>
@@ -8006,26 +10253,29 @@
         <v>174</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="I30" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[28] = new TableColDefEx("Initials", typeof(String), "initials","Adprop");</v>
+        <v>collist[28] = new TableColDefEx("POBox", typeof(String), "postofficebox","Adprop");</v>
       </c>
       <c r="J30" t="str">
         <f>CONCATENATE("[",C30,"] [",A30,"](",D30,") ",E30,",")</f>
-        <v>[Initials] [nvarchar](32) NULL,</v>
+        <v>[POBox] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>55</v>
+      </c>
+      <c r="D31">
+        <v>32</v>
       </c>
       <c r="E31" t="s">
         <v>115</v>
@@ -8034,29 +10284,32 @@
         <v>29</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="H31" s="19" t="s">
-        <v>157</v>
+        <v>174</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>195</v>
       </c>
       <c r="I31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[29] = new TableColDefEx("LastBadPasswordAttempt", typeof(DateTime), "badpasswordtime","filetime");</v>
+        <v>collist[29] = new TableColDefEx("PostalCode", typeof(String), "postalcode","Adprop");</v>
       </c>
       <c r="J31" t="str">
-        <f>CONCATENATE("[",C31,"] [",A31,"] ",E31,",")</f>
-        <v>[LastBadPasswordAttempt] [datetime] NULL,</v>
+        <f>CONCATENATE("[",C31,"] [",A31,"](",D31,") ",E31,",")</f>
+        <v>[PostalCode] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" t="s">
-        <v>36</v>
+        <v>83</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32">
+        <v>64</v>
       </c>
       <c r="E32" t="s">
         <v>115</v>
@@ -8065,29 +10318,32 @@
         <v>30</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="H32" s="19" t="s">
-        <v>200</v>
+        <v>174</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="I32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[30] = new TableColDefEx("LastLogonDate", typeof(DateTime), "lastlogon","filetime");</v>
+        <v>collist[30] = new TableColDefEx("State", typeof(String), "st","Adprop");</v>
       </c>
       <c r="J32" t="str">
-        <f>CONCATENATE("[",C32,"] [",A32,"] ",E32,",")</f>
-        <v>[LastLogonDate] [datetime] NULL,</v>
+        <f>CONCATENATE("[",C32,"] [",A32,"](",D32,") ",E32,",")</f>
+        <v>[State] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>37</v>
+        <v>83</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33">
+        <v>160</v>
       </c>
       <c r="E33" t="s">
         <v>115</v>
@@ -8096,29 +10352,32 @@
         <v>31</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>167</v>
+        <v>198</v>
       </c>
       <c r="I33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[31] = new TableColDefEx("LockedOut", typeof(Boolean), "LOCKOUT","UAC");</v>
+        <v>collist[31] = new TableColDefEx("StreetAddress", typeof(String), "streetaddress","Adprop");</v>
       </c>
       <c r="J33" t="str">
-        <f>CONCATENATE("[",C33,"] [",A33,"] ",E33,",")</f>
-        <v>[LockedOut] [bit] NULL,</v>
+        <f>CONCATENATE("[",C33,"] [",A33,"](",D33,") ",E33,",")</f>
+        <v>[StreetAddress] [nvarchar](160) NULL,</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>201</v>
+        <v>83</v>
+      </c>
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34">
+        <v>256</v>
       </c>
       <c r="E34" t="s">
         <v>115</v>
@@ -8129,16 +10388,16 @@
       <c r="G34" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H34" s="18" t="s">
-        <v>147</v>
+      <c r="H34" s="15" t="s">
+        <v>126</v>
       </c>
       <c r="I34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[32] = new TableColDefEx("LogonCount", typeof(Int32), "logoncount","Adprop");</v>
+        <v>collist[32] = new TableColDefEx("Surname", typeof(String), "sn","Adprop");</v>
       </c>
       <c r="J34" t="str">
-        <f>CONCATENATE("[",C34,"] [",A34,"] ",E34,",")</f>
-        <v>[LogonCount] [int] NULL,</v>
+        <f>CONCATENATE("[",C34,"] [",A34,"](",D34,") ",E34,",")</f>
+        <v>[Surname] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -8148,8 +10407,8 @@
       <c r="B35" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>38</v>
+      <c r="C35" t="s">
+        <v>64</v>
       </c>
       <c r="D35">
         <v>128</v>
@@ -8164,1077 +10423,25 @@
         <v>174</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="I35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>collist[33] = new TableColDefEx("LogonWorkstations", typeof(String), "userworkstations","Adprop");</v>
+        <v>collist[33] = new TableColDefEx("Title", typeof(String), "title","Adprop");</v>
       </c>
       <c r="J35" t="str">
         <f>CONCATENATE("[",C35,"] [",A35,"](",D35,") ",E35,",")</f>
-        <v>[LogonWorkstations] [nvarchar](128) NULL,</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36">
-        <v>256</v>
-      </c>
-      <c r="E36" t="s">
-        <v>115</v>
-      </c>
-      <c r="F36" s="6">
-        <v>34</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H36" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="I36" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[34] = new TableColDefEx("Manager", typeof(String), "manager","Adprop");</v>
-      </c>
-      <c r="J36" t="str">
-        <f>CONCATENATE("[",C36,"] [",A36,"](",D36,") ",E36,",")</f>
-        <v>[Manager] [nvarchar](256) NULL,</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E37" t="s">
-        <v>115</v>
-      </c>
-      <c r="F37" s="6">
-        <v>35</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H37" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="I37" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[35] = new TableColDefEx("MNSLogonAccount", typeof(Boolean), "MNS_LOGON_ACCOUNT","UAC");</v>
-      </c>
-      <c r="J37" t="str">
-        <f>CONCATENATE("[",C37,"] [",A37,"] ",E37,",")</f>
-        <v>[MNSLogonAccount] [bit] NULL,</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38">
-        <v>32</v>
-      </c>
-      <c r="E38" t="s">
-        <v>115</v>
-      </c>
-      <c r="F38" s="6">
-        <v>36</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="I38" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[36] = new TableColDefEx("MobilePhone", typeof(String), "mobile","Adprop");</v>
-      </c>
-      <c r="J38" t="str">
-        <f>CONCATENATE("[",C38,"] [",A38,"](",D38,") ",E38,",")</f>
-        <v>[MobilePhone] [nvarchar](32) NULL,</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" t="s">
-        <v>115</v>
-      </c>
-      <c r="F39" s="6">
-        <v>37</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="I39" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[37] = new TableColDefEx("Modified", typeof(DateTime), "whenchanged","Adprop");</v>
-      </c>
-      <c r="J39" t="str">
-        <f>CONCATENATE("[",C39,"] [",A39,"] ",E39,",")</f>
-        <v>[Modified] [datetime] NULL,</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40">
-        <v>256</v>
-      </c>
-      <c r="E40" t="s">
-        <v>115</v>
-      </c>
-      <c r="F40" s="6">
-        <v>38</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H40" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="I40" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[38] = new TableColDefEx("Name", typeof(String), "name","Adprop");</v>
-      </c>
-      <c r="J40" t="str">
-        <f>CONCATENATE("[",C40,"] [",A40,"](",D40,") ",E40,",")</f>
-        <v>[Name] [nvarchar](256) NULL,</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41">
-        <v>128</v>
-      </c>
-      <c r="E41" t="s">
-        <v>115</v>
-      </c>
-      <c r="F41" s="6">
-        <v>39</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H41" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="I41" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[39] = new TableColDefEx("ObjectCategory", typeof(String), "objectcategory","Adprop");</v>
-      </c>
-      <c r="J41" t="str">
-        <f>CONCATENATE("[",C41,"] [",A41,"](",D41,") ",E41,",")</f>
-        <v>[ObjectCategory] [nvarchar](128) NULL,</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42">
-        <v>64</v>
-      </c>
-      <c r="E42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F42" s="6">
-        <v>40</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="I42" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[40] = new TableColDefEx("ObjectClass", typeof(String), "SchemaClassName","ObjClass");</v>
-      </c>
-      <c r="J42" t="str">
-        <f>CONCATENATE("[",C42,"] [",A42,"](",D42,") ",E42,",")</f>
-        <v>[ObjectClass] [nvarchar](64) NULL,</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" t="s">
-        <v>47</v>
-      </c>
-      <c r="E43" t="s">
-        <v>116</v>
-      </c>
-      <c r="F43" s="6">
-        <v>41</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="I43" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[41] = new TableColDefEx("ObjectGUID", typeof(Guid), "Guid","ObjGuid");</v>
-      </c>
-      <c r="J43" t="str">
-        <f>CONCATENATE("[",C43,"] [",A43,"] ",E43,",")</f>
-        <v>[ObjectGUID] [uniqueidentifier] NOT NULL,</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44">
-        <v>128</v>
-      </c>
-      <c r="E44" t="s">
-        <v>115</v>
-      </c>
-      <c r="F44" s="6">
-        <v>42</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="I44" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[42] = new TableColDefEx("Office", typeof(String), "physicalDeliveryOfficeName","Adprop");</v>
-      </c>
-      <c r="J44" t="str">
-        <f>CONCATENATE("[",C44,"] [",A44,"](",D44,") ",E44,",")</f>
-        <v>[Office] [nvarchar](128) NULL,</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45">
-        <v>32</v>
-      </c>
-      <c r="E45" t="s">
-        <v>115</v>
-      </c>
-      <c r="F45" s="6">
-        <v>43</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H45" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="I45" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[43] = new TableColDefEx("OfficePhone", typeof(String), "telephonenumber","Adprop");</v>
-      </c>
-      <c r="J45" t="str">
-        <f>CONCATENATE("[",C45,"] [",A45,"](",D45,") ",E45,",")</f>
-        <v>[OfficePhone] [nvarchar](32) NULL,</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" t="s">
-        <v>69</v>
-      </c>
-      <c r="D46">
-        <v>32</v>
-      </c>
-      <c r="E46" t="s">
-        <v>115</v>
-      </c>
-      <c r="F46" s="6">
-        <v>44</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H46" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="I46" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[44] = new TableColDefEx("Pager", typeof(String), "pager","Adprop");</v>
-      </c>
-      <c r="J46" t="str">
-        <f>CONCATENATE("[",C46,"] [",A46,"](",D46,") ",E46,",")</f>
-        <v>[Pager] [nvarchar](32) NULL,</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47" t="s">
-        <v>80</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E47" t="s">
-        <v>115</v>
-      </c>
-      <c r="F47" s="6">
-        <v>45</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="I47" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[45] = new TableColDefEx("PasswordExpired", typeof(Boolean), "PASSWORD_EXPIRED","UAC");</v>
-      </c>
-      <c r="J47" t="str">
-        <f>CONCATENATE("[",C47,"] [",A47,"] ",E47,",")</f>
-        <v>[PasswordExpired] [bit] NULL,</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" t="s">
-        <v>51</v>
-      </c>
-      <c r="E48" t="s">
-        <v>115</v>
-      </c>
-      <c r="F48" s="6">
-        <v>46</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="H48" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="I48" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[46] = new TableColDefEx("PasswordLastSet", typeof(DateTime), "pwdlastset","filetime");</v>
-      </c>
-      <c r="J48" t="str">
-        <f>CONCATENATE("[",C48,"] [",A48,"] ",E48,",")</f>
-        <v>[PasswordLastSet] [datetime] NULL,</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" t="s">
-        <v>80</v>
-      </c>
-      <c r="C49" t="s">
-        <v>52</v>
-      </c>
-      <c r="E49" t="s">
-        <v>115</v>
-      </c>
-      <c r="F49" s="6">
-        <v>47</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H49" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="I49" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[47] = new TableColDefEx("PasswordNeverExpires", typeof(Boolean), "DONT_EXPIRE_PASSWD","UAC");</v>
-      </c>
-      <c r="J49" t="str">
-        <f>CONCATENATE("[",C49,"] [",A49,"] ",E49,",")</f>
-        <v>[PasswordNeverExpires] [bit] NULL,</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" t="s">
-        <v>80</v>
-      </c>
-      <c r="C50" t="s">
-        <v>53</v>
-      </c>
-      <c r="E50" t="s">
-        <v>115</v>
-      </c>
-      <c r="F50" s="6">
-        <v>48</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H50" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="I50" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[48] = new TableColDefEx("PasswordNotRequired", typeof(Boolean), "PASSWD_NOTREQD","UAC");</v>
-      </c>
-      <c r="J50" t="str">
-        <f>CONCATENATE("[",C50,"] [",A50,"] ",E50,",")</f>
-        <v>[PasswordNotRequired] [bit] NULL,</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>11</v>
-      </c>
-      <c r="B51" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D51">
-        <v>32</v>
-      </c>
-      <c r="E51" t="s">
-        <v>115</v>
-      </c>
-      <c r="F51" s="6">
-        <v>49</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H51" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="I51" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[49] = new TableColDefEx("POBox", typeof(String), "postofficebox","Adprop");</v>
-      </c>
-      <c r="J51" t="str">
-        <f>CONCATENATE("[",C51,"] [",A51,"](",D51,") ",E51,",")</f>
-        <v>[POBox] [nvarchar](32) NULL,</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>11</v>
-      </c>
-      <c r="B52" t="s">
-        <v>83</v>
-      </c>
-      <c r="C52" t="s">
-        <v>55</v>
-      </c>
-      <c r="D52">
-        <v>32</v>
-      </c>
-      <c r="E52" t="s">
-        <v>115</v>
-      </c>
-      <c r="F52" s="6">
-        <v>50</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H52" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="I52" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[50] = new TableColDefEx("PostalCode", typeof(String), "postalcode","Adprop");</v>
-      </c>
-      <c r="J52" t="str">
-        <f>CONCATENATE("[",C52,"] [",A52,"](",D52,") ",E52,",")</f>
-        <v>[PostalCode] [nvarchar](32) NULL,</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>8</v>
-      </c>
-      <c r="B53" t="s">
-        <v>82</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="D53">
-        <v>128</v>
-      </c>
-      <c r="E53" t="s">
-        <v>115</v>
-      </c>
-      <c r="F53" s="6">
-        <v>51</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H53" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="I53" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[51] = new TableColDefEx("PrimaryGroupID", typeof(Int32), "primarygroupid","Adprop");</v>
-      </c>
-      <c r="J53" t="str">
-        <f>CONCATENATE("[",C53,"] [",A53,"] ",E53,",")</f>
-        <v>[PrimaryGroupID] [int] NULL,</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>11</v>
-      </c>
-      <c r="B54" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54" t="s">
-        <v>56</v>
-      </c>
-      <c r="D54">
-        <v>128</v>
-      </c>
-      <c r="E54" t="s">
-        <v>115</v>
-      </c>
-      <c r="F54" s="6">
-        <v>52</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H54" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="I54" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[52] = new TableColDefEx("ProfilePath", typeof(String), "profilepath","Adprop");</v>
-      </c>
-      <c r="J54" t="str">
-        <f>CONCATENATE("[",C54,"] [",A54,"](",D54,") ",E54,",")</f>
-        <v>[ProfilePath] [nvarchar](128) NULL,</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>11</v>
-      </c>
-      <c r="B55" t="s">
-        <v>83</v>
-      </c>
-      <c r="C55" t="s">
-        <v>57</v>
-      </c>
-      <c r="D55">
-        <v>128</v>
-      </c>
-      <c r="E55" t="s">
-        <v>115</v>
-      </c>
-      <c r="F55" s="6">
-        <v>53</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="I55" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[53] = new TableColDefEx("SamAccountName", typeof(String), "samaccountname","Adprop");</v>
-      </c>
-      <c r="J55" t="str">
-        <f>CONCATENATE("[",C55,"] [",A55,"](",D55,") ",E55,",")</f>
-        <v>[SamAccountName] [nvarchar](128) NULL,</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>11</v>
-      </c>
-      <c r="B56" t="s">
-        <v>83</v>
-      </c>
-      <c r="C56" t="s">
-        <v>58</v>
-      </c>
-      <c r="D56">
-        <v>256</v>
-      </c>
-      <c r="E56" t="s">
-        <v>115</v>
-      </c>
-      <c r="F56" s="6">
-        <v>54</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H56" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="I56" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[54] = new TableColDefEx("ScriptPath", typeof(String), "scriptpath","Adprop");</v>
-      </c>
-      <c r="J56" t="str">
-        <f>CONCATENATE("[",C56,"] [",A56,"](",D56,") ",E56,",")</f>
-        <v>[ScriptPath] [nvarchar](256) NULL,</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>11</v>
-      </c>
-      <c r="B57" t="s">
-        <v>83</v>
-      </c>
-      <c r="C57" t="s">
-        <v>59</v>
-      </c>
-      <c r="D57">
-        <v>128</v>
-      </c>
-      <c r="E57" t="s">
-        <v>116</v>
-      </c>
-      <c r="F57" s="6">
-        <v>55</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H57" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="I57" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[55] = new TableColDefEx("SID", typeof(String), "objectsid","SID");</v>
-      </c>
-      <c r="J57" t="str">
-        <f>CONCATENATE("[",C57,"] [",A57,"](",D57,") ",E57,",")</f>
-        <v>[SID] [nvarchar](128) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" t="s">
-        <v>80</v>
-      </c>
-      <c r="C58" t="s">
-        <v>60</v>
-      </c>
-      <c r="E58" t="s">
-        <v>115</v>
-      </c>
-      <c r="F58" s="6">
-        <v>56</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H58" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="I58" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[56] = new TableColDefEx("SmartcardLogonRequired", typeof(Boolean), "SMARTCARD_REQUIRED","UAC");</v>
-      </c>
-      <c r="J58" t="str">
-        <f>CONCATENATE("[",C58,"] [",A58,"] ",E58,",")</f>
-        <v>[SmartcardLogonRequired] [bit] NULL,</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>11</v>
-      </c>
-      <c r="B59" t="s">
-        <v>83</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D59">
-        <v>64</v>
-      </c>
-      <c r="E59" t="s">
-        <v>115</v>
-      </c>
-      <c r="F59" s="6">
-        <v>57</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H59" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I59" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[57] = new TableColDefEx("State", typeof(String), "st","Adprop");</v>
-      </c>
-      <c r="J59" t="str">
-        <f>CONCATENATE("[",C59,"] [",A59,"](",D59,") ",E59,",")</f>
-        <v>[State] [nvarchar](64) NULL,</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>11</v>
-      </c>
-      <c r="B60" t="s">
-        <v>83</v>
-      </c>
-      <c r="C60" t="s">
-        <v>62</v>
-      </c>
-      <c r="D60">
-        <v>160</v>
-      </c>
-      <c r="E60" t="s">
-        <v>115</v>
-      </c>
-      <c r="F60" s="6">
-        <v>58</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H60" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="I60" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[58] = new TableColDefEx("StreetAddress", typeof(String), "streetaddress","Adprop");</v>
-      </c>
-      <c r="J60" t="str">
-        <f>CONCATENATE("[",C60,"] [",A60,"](",D60,") ",E60,",")</f>
-        <v>[StreetAddress] [nvarchar](160) NULL,</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>11</v>
-      </c>
-      <c r="B61" t="s">
-        <v>83</v>
-      </c>
-      <c r="C61" t="s">
-        <v>63</v>
-      </c>
-      <c r="D61">
-        <v>256</v>
-      </c>
-      <c r="E61" t="s">
-        <v>115</v>
-      </c>
-      <c r="F61" s="6">
-        <v>59</v>
-      </c>
-      <c r="G61" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H61" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="I61" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[59] = new TableColDefEx("Surname", typeof(String), "sn","Adprop");</v>
-      </c>
-      <c r="J61" t="str">
-        <f>CONCATENATE("[",C61,"] [",A61,"](",D61,") ",E61,",")</f>
-        <v>[Surname] [nvarchar](256) NULL,</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>11</v>
-      </c>
-      <c r="B62" t="s">
-        <v>83</v>
-      </c>
-      <c r="C62" t="s">
-        <v>64</v>
-      </c>
-      <c r="D62">
-        <v>128</v>
-      </c>
-      <c r="E62" t="s">
-        <v>115</v>
-      </c>
-      <c r="F62" s="6">
-        <v>60</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H62" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="I62" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[60] = new TableColDefEx("Title", typeof(String), "title","Adprop");</v>
-      </c>
-      <c r="J62" t="str">
-        <f>CONCATENATE("[",C62,"] [",A62,"](",D62,") ",E62,",")</f>
         <v>[Title] [nvarchar](128) NULL,</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63" t="s">
-        <v>80</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E63" t="s">
-        <v>115</v>
-      </c>
-      <c r="F63" s="6">
-        <v>61</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H63" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="I63" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[61] = new TableColDefEx("TrustedForDelegation", typeof(Boolean), "TRUSTED_FOR_DELEGATION","UAC");</v>
-      </c>
-      <c r="J63" t="str">
-        <f t="shared" ref="J63:J67" si="1">CONCATENATE("[",C63,"] [",A63,"] ",E63,",")</f>
-        <v>[TrustedForDelegation] [bit] NULL,</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64" t="s">
-        <v>80</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E64" t="s">
-        <v>115</v>
-      </c>
-      <c r="F64" s="6">
-        <v>62</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H64" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="I64" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[62] = new TableColDefEx("TrustedToAuthForDelegation", typeof(Boolean), "TRUSTED_TO_AUTH_FOR_DELEGATION","UAC");</v>
-      </c>
-      <c r="J64" t="str">
-        <f t="shared" si="1"/>
-        <v>[TrustedToAuthForDelegation] [bit] NULL,</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>5</v>
-      </c>
-      <c r="B65" t="s">
-        <v>80</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E65" t="s">
-        <v>115</v>
-      </c>
-      <c r="F65" s="6">
-        <v>63</v>
-      </c>
-      <c r="G65" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H65" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="I65" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[63] = new TableColDefEx("UseDESKeyOnly", typeof(Boolean), "USE_DES_KEY_ONLY","UAC");</v>
-      </c>
-      <c r="J65" t="str">
-        <f t="shared" si="1"/>
-        <v>[UseDESKeyOnly] [bit] NULL,</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>11</v>
-      </c>
-      <c r="B66" t="s">
-        <v>83</v>
-      </c>
-      <c r="C66" t="s">
-        <v>68</v>
-      </c>
-      <c r="D66">
-        <v>256</v>
-      </c>
-      <c r="E66" t="s">
-        <v>115</v>
-      </c>
-      <c r="F66" s="6">
-        <v>64</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H66" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="I66" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[64] = new TableColDefEx("UserPrincipalName", typeof(String), "userprincipalname","Adprop");</v>
-      </c>
-      <c r="J66" t="str">
-        <f>CONCATENATE("[",C66,"] [",A66,"](",D66,") ",E66,",")</f>
-        <v>[UserPrincipalName] [nvarchar](256) NULL,</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>8</v>
-      </c>
-      <c r="B67" t="s">
-        <v>82</v>
-      </c>
-      <c r="C67" t="s">
-        <v>99</v>
-      </c>
-      <c r="E67" t="s">
-        <v>115</v>
-      </c>
-      <c r="F67" s="6">
-        <v>65</v>
-      </c>
-      <c r="G67" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H67" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="I67" s="1" t="str">
-        <f t="shared" ref="I67" si="2">CONCATENATE("collist[",F67,"] = new TableColDefEx(""",C67,""", typeof(",B67,"), """,H67,""",""",G67,""");")</f>
-        <v>collist[65] = new TableColDefEx("userAccountControl", typeof(Int32), "useraccountcontrol","Adprop");</v>
-      </c>
-      <c r="J67" t="str">
-        <f t="shared" si="1"/>
-        <v>[userAccountControl] [int] NULL,</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J68"/>
+  <autoFilter ref="A1:J36"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
@@ -10612,11 +11819,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
A few minor changes
</commit_message>
<xml_diff>
--- a/GetADobjects/AD_DW_Users table map to .net V4.xlsx
+++ b/GetADobjects/AD_DW_Users table map to .net V4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" tabRatio="625" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" tabRatio="625" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Groups!$A$1:$L$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Groups (2)'!$A$1:$J$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Users!$A$1:$L$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Users (2)'!$A$1:$J$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Users (2)'!$A$1:$J$60</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -655,7 +655,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -679,15 +679,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -697,18 +690,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,7 +707,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
@@ -752,11 +733,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7011,7 +6987,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7060,13 +7038,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="D2">
+        <v>128</v>
       </c>
       <c r="E2" t="s">
         <v>115</v>
@@ -7075,29 +7056,32 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>145</v>
+        <v>173</v>
+      </c>
+      <c r="H2" t="s">
+        <v>176</v>
       </c>
       <c r="I2" s="1" t="str">
         <f>CONCATENATE("collist[",F2,"] = new TableColDefEx(""",C2,""", typeof(",B2,"), """,H2,""",""",G2,""");")</f>
-        <v>collist[0] = new TableColDefEx("AccountExpirationDate", typeof(DateTime), "accountexpires","filetime");</v>
+        <v>collist[0] = new TableColDefEx("GivenName", typeof(String), "givenname","Adprop");</v>
       </c>
       <c r="J2" t="str">
-        <f>CONCATENATE("[",C2,"] [",A2,"] ",E2,",")</f>
-        <v>[AccountExpirationDate] [datetime] NULL,</v>
+        <f>CONCATENATE("[",C2,"] [",A2,"](",D2,") ",E2,",")</f>
+        <v>[GivenName] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>32</v>
       </c>
       <c r="E3" t="s">
         <v>115</v>
@@ -7106,29 +7090,32 @@
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>168</v>
+        <v>173</v>
+      </c>
+      <c r="H3" t="s">
+        <v>182</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I66" si="0">CONCATENATE("collist[",F3,"] = new TableColDefEx(""",C3,""", typeof(",B3,"), """,H3,""",""",G3,""");")</f>
-        <v>collist[1] = new TableColDefEx("AccountLockoutTime", typeof(DateTime), "lockouttime","filetime");</v>
+        <f>CONCATENATE("collist[",F3,"] = new TableColDefEx(""",C3,""", typeof(",B3,"), """,H3,""",""",G3,""");")</f>
+        <v>collist[1] = new TableColDefEx("Initials", typeof(String), "initials","Adprop");</v>
       </c>
       <c r="J3" t="str">
-        <f>CONCATENATE("[",C3,"] [",A3,"] ",E3,",")</f>
-        <v>[AccountLockoutTime] [datetime] NULL,</v>
+        <f>CONCATENATE("[",C3,"] [",A3,"](",D3,") ",E3,",")</f>
+        <v>[Initials] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>6</v>
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4">
+        <v>256</v>
       </c>
       <c r="E4" t="s">
         <v>115</v>
@@ -7137,29 +7124,32 @@
         <v>2</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>105</v>
+        <v>173</v>
+      </c>
+      <c r="H4" t="s">
+        <v>126</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[2] = new TableColDefEx("AccountNotDelegated", typeof(Boolean), "NOT_DELEGATED","UAC");</v>
+        <f>CONCATENATE("collist[",F4,"] = new TableColDefEx(""",C4,""", typeof(",B4,"), """,H4,""",""",G4,""");")</f>
+        <v>collist[2] = new TableColDefEx("Surname", typeof(String), "sn","Adprop");</v>
       </c>
       <c r="J4" t="str">
-        <f>CONCATENATE("[",C4,"] [",A4,"] ",E4,",")</f>
-        <v>[AccountNotDelegated] [bit] NULL,</v>
+        <f>CONCATENATE("[",C4,"] [",A4,"](",D4,") ",E4,",")</f>
+        <v>[Surname] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>128</v>
       </c>
       <c r="E5" t="s">
         <v>115</v>
@@ -7168,29 +7158,32 @@
         <v>3</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>167</v>
+        <v>173</v>
+      </c>
+      <c r="H5" t="s">
+        <v>141</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[3] = new TableColDefEx("AllowReversiblePasswordEncryption", typeof(Boolean), "ENCRYPTED_TEXT_PWD_ALLOWED","UAC");</v>
+        <f>CONCATENATE("collist[",F5,"] = new TableColDefEx(""",C5,""", typeof(",B5,"), """,H5,""",""",G5,""");")</f>
+        <v>collist[3] = new TableColDefEx("DisplayName", typeof(String), "displayname","Adprop");</v>
       </c>
       <c r="J5" t="str">
-        <f>CONCATENATE("[",C5,"] [",A5,"] ",E5,",")</f>
-        <v>[AllowReversiblePasswordEncryption] [bit] NULL,</v>
+        <f>CONCATENATE("[",C5,"] [",A5,"](",D5,") ",E5,",")</f>
+        <v>[DisplayName] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>256</v>
       </c>
       <c r="E6" t="s">
         <v>115</v>
@@ -7201,27 +7194,30 @@
       <c r="G6" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>150</v>
+      <c r="H6" t="s">
+        <v>120</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[4] = new TableColDefEx("BadLogonCount", typeof(Int32), "badpwdcount","Adprop");</v>
+        <f>CONCATENATE("collist[",F6,"] = new TableColDefEx(""",C6,""", typeof(",B6,"), """,H6,""",""",G6,""");")</f>
+        <v>collist[4] = new TableColDefEx("Description", typeof(String), "description","Adprop");</v>
       </c>
       <c r="J6" t="str">
-        <f>CONCATENATE("[",C6,"] [",A6,"] ",E6,",")</f>
-        <v>[BadLogonCount] [int] NULL,</v>
+        <f>CONCATENATE("[",C6,"] [",A6,"](",D6,") ",E6,",")</f>
+        <v>[Description] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
+        <v>83</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7">
+        <v>128</v>
       </c>
       <c r="E7" t="s">
         <v>115</v>
@@ -7230,18 +7226,18 @@
         <v>5</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>163</v>
+        <v>173</v>
+      </c>
+      <c r="H7" t="s">
+        <v>91</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[5] = new TableColDefEx("CannotChangePassword", typeof(Boolean), "PASSWD_CANT_CHANGE","UAC");</v>
+        <f>CONCATENATE("collist[",F7,"] = new TableColDefEx(""",C7,""", typeof(",B7,"), """,H7,""",""",G7,""");")</f>
+        <v>collist[5] = new TableColDefEx("Office", typeof(String), "physicalDeliveryOfficeName","Adprop");</v>
       </c>
       <c r="J7" t="str">
-        <f>CONCATENATE("[",C7,"] [",A7,"] ",E7,",")</f>
-        <v>[CannotChangePassword] [bit] NULL,</v>
+        <f>CONCATENATE("[",C7,"] [",A7,"](",D7,") ",E7,",")</f>
+        <v>[Office] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -7252,10 +7248,10 @@
         <v>83</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="D8">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
         <v>115</v>
@@ -7266,16 +7262,16 @@
       <c r="G8" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H8" s="15" t="s">
-        <v>96</v>
+      <c r="H8" t="s">
+        <v>181</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[6] = new TableColDefEx("City", typeof(String), "l","Adprop");</v>
+        <f>CONCATENATE("collist[",F8,"] = new TableColDefEx(""",C8,""", typeof(",B8,"), """,H8,""",""",G8,""");")</f>
+        <v>collist[6] = new TableColDefEx("OfficePhone", typeof(String), "telephonenumber","Adprop");</v>
       </c>
       <c r="J8" t="str">
         <f>CONCATENATE("[",C8,"] [",A8,"](",D8,") ",E8,",")</f>
-        <v>[City] [nvarchar](128) NULL,</v>
+        <v>[OfficePhone] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -7286,7 +7282,7 @@
         <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D9">
         <v>256</v>
@@ -7300,16 +7296,16 @@
       <c r="G9" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H9" s="15" t="s">
-        <v>152</v>
+      <c r="H9" t="s">
+        <v>123</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[7] = new TableColDefEx("CN", typeof(String), "cn","Adprop");</v>
+        <f>CONCATENATE("collist[",F9,"] = new TableColDefEx(""",C9,""", typeof(",B9,"), """,H9,""",""",G9,""");")</f>
+        <v>collist[7] = new TableColDefEx("EmailAddress", typeof(String), "mail","Adprop");</v>
       </c>
       <c r="J9" t="str">
         <f>CONCATENATE("[",C9,"] [",A9,"](",D9,") ",E9,",")</f>
-        <v>[CN] [nvarchar](256) NULL,</v>
+        <v>[EmailAddress] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -7319,8 +7315,8 @@
       <c r="B10" t="s">
         <v>83</v>
       </c>
-      <c r="C10" t="s">
-        <v>14</v>
+      <c r="C10" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="D10">
         <v>128</v>
@@ -7334,16 +7330,16 @@
       <c r="G10" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H10" s="15" t="s">
-        <v>180</v>
+      <c r="H10" t="s">
+        <v>191</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[8] = new TableColDefEx("Company", typeof(String), "company","Adprop");</v>
+        <f>CONCATENATE("collist[",F10,"] = new TableColDefEx(""",C10,""", typeof(",B10,"), """,H10,""",""",G10,""");")</f>
+        <v>collist[8] = new TableColDefEx("HomePage", typeof(String), "wwwhomepage","Adprop");</v>
       </c>
       <c r="J10" t="str">
         <f>CONCATENATE("[",C10,"] [",A10,"](",D10,") ",E10,",")</f>
-        <v>[Company] [nvarchar](128) NULL,</v>
+        <v>[HomePage] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -7353,11 +7349,11 @@
       <c r="B11" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>15</v>
+      <c r="C11" t="s">
+        <v>62</v>
       </c>
       <c r="D11">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="E11" t="s">
         <v>115</v>
@@ -7368,27 +7364,30 @@
       <c r="G11" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H11" s="15" t="s">
-        <v>89</v>
+      <c r="H11" t="s">
+        <v>197</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[9] = new TableColDefEx("Country", typeof(String), "co","Adprop");</v>
+        <f>CONCATENATE("collist[",F11,"] = new TableColDefEx(""",C11,""", typeof(",B11,"), """,H11,""",""",G11,""");")</f>
+        <v>collist[9] = new TableColDefEx("StreetAddress", typeof(String), "streetaddress","Adprop");</v>
       </c>
       <c r="J11" t="str">
         <f>CONCATENATE("[",C11,"] [",A11,"](",D11,") ",E11,",")</f>
-        <v>[Country] [nvarchar](128) NULL,</v>
+        <v>[StreetAddress] [nvarchar](160) NULL,</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>16</v>
+        <v>54</v>
+      </c>
+      <c r="D12">
+        <v>32</v>
       </c>
       <c r="E12" t="s">
         <v>115</v>
@@ -7399,16 +7398,16 @@
       <c r="G12" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>183</v>
+      <c r="H12" t="s">
+        <v>193</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[10] = new TableColDefEx("Created", typeof(DateTime), "whencreated","Adprop");</v>
+        <f>CONCATENATE("collist[",F12,"] = new TableColDefEx(""",C12,""", typeof(",B12,"), """,H12,""",""",G12,""");")</f>
+        <v>collist[10] = new TableColDefEx("POBox", typeof(String), "postofficebox","Adprop");</v>
       </c>
       <c r="J12" t="str">
-        <f>CONCATENATE("[",C12,"] [",A12,"] ",E12,",")</f>
-        <v>[Created] [datetime] NULL,</v>
+        <f>CONCATENATE("[",C12,"] [",A12,"](",D12,") ",E12,",")</f>
+        <v>[POBox] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -7418,8 +7417,8 @@
       <c r="B13" t="s">
         <v>83</v>
       </c>
-      <c r="C13" t="s">
-        <v>17</v>
+      <c r="C13" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="D13">
         <v>128</v>
@@ -7433,16 +7432,16 @@
       <c r="G13" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H13" s="15" t="s">
-        <v>185</v>
+      <c r="H13" t="s">
+        <v>96</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[11] = new TableColDefEx("Department", typeof(String), "department","Adprop");</v>
+        <f>CONCATENATE("collist[",F13,"] = new TableColDefEx(""",C13,""", typeof(",B13,"), """,H13,""",""",G13,""");")</f>
+        <v>collist[11] = new TableColDefEx("City", typeof(String), "l","Adprop");</v>
       </c>
       <c r="J13" t="str">
         <f>CONCATENATE("[",C13,"] [",A13,"](",D13,") ",E13,",")</f>
-        <v>[Department] [nvarchar](128) NULL,</v>
+        <v>[City] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -7452,11 +7451,11 @@
       <c r="B14" t="s">
         <v>83</v>
       </c>
-      <c r="C14" t="s">
-        <v>18</v>
+      <c r="C14" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="D14">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
         <v>115</v>
@@ -7467,16 +7466,16 @@
       <c r="G14" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H14" s="15" t="s">
-        <v>120</v>
+      <c r="H14" t="s">
+        <v>90</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[12] = new TableColDefEx("Description", typeof(String), "description","Adprop");</v>
+        <f>CONCATENATE("collist[",F14,"] = new TableColDefEx(""",C14,""", typeof(",B14,"), """,H14,""",""",G14,""");")</f>
+        <v>collist[12] = new TableColDefEx("State", typeof(String), "st","Adprop");</v>
       </c>
       <c r="J14" t="str">
         <f>CONCATENATE("[",C14,"] [",A14,"](",D14,") ",E14,",")</f>
-        <v>[Description] [nvarchar](256) NULL,</v>
+        <v>[State] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -7487,10 +7486,10 @@
         <v>83</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D15">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
         <v>115</v>
@@ -7501,16 +7500,16 @@
       <c r="G15" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H15" s="15" t="s">
-        <v>141</v>
+      <c r="H15" t="s">
+        <v>194</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[13] = new TableColDefEx("DisplayName", typeof(String), "displayname","Adprop");</v>
+        <f>CONCATENATE("collist[",F15,"] = new TableColDefEx(""",C15,""", typeof(",B15,"), """,H15,""",""",G15,""");")</f>
+        <v>collist[13] = new TableColDefEx("PostalCode", typeof(String), "postalcode","Adprop");</v>
       </c>
       <c r="J15" t="str">
         <f>CONCATENATE("[",C15,"] [",A15,"](",D15,") ",E15,",")</f>
-        <v>[DisplayName] [nvarchar](128) NULL,</v>
+        <v>[PostalCode] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -7520,11 +7519,11 @@
       <c r="B16" t="s">
         <v>83</v>
       </c>
-      <c r="C16" t="s">
-        <v>20</v>
+      <c r="C16" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="D16">
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="E16" t="s">
         <v>115</v>
@@ -7535,16 +7534,16 @@
       <c r="G16" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H16" s="15" t="s">
-        <v>140</v>
+      <c r="H16" t="s">
+        <v>89</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[14] = new TableColDefEx("DistinguishedName", typeof(String), "distinguishedname","Adprop");</v>
+        <f>CONCATENATE("collist[",F16,"] = new TableColDefEx(""",C16,""", typeof(",B16,"), """,H16,""",""",G16,""");")</f>
+        <v>collist[14] = new TableColDefEx("Country", typeof(String), "co","Adprop");</v>
       </c>
       <c r="J16" t="str">
         <f>CONCATENATE("[",C16,"] [",A16,"](",D16,") ",E16,",")</f>
-        <v>[DistinguishedName] [nvarchar](512) NULL,</v>
+        <v>[Country] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -7555,10 +7554,10 @@
         <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D17">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
         <v>115</v>
@@ -7569,27 +7568,30 @@
       <c r="G17" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H17" s="15" t="s">
-        <v>187</v>
+      <c r="H17" t="s">
+        <v>186</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[15] = new TableColDefEx("Division", typeof(String), "division","Adprop");</v>
+        <f>CONCATENATE("collist[",F17,"] = new TableColDefEx(""",C17,""", typeof(",B17,"), """,H17,""",""",G17,""");")</f>
+        <v>collist[15] = new TableColDefEx("HomePhone", typeof(String), "homephone","Adprop");</v>
       </c>
       <c r="J17" t="str">
         <f>CONCATENATE("[",C17,"] [",A17,"](",D17,") ",E17,",")</f>
-        <v>[Division] [nvarchar](128) NULL,</v>
+        <v>[HomePhone] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>22</v>
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18">
+        <v>32</v>
       </c>
       <c r="E18" t="s">
         <v>115</v>
@@ -7598,18 +7600,18 @@
         <v>16</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>107</v>
+        <v>173</v>
+      </c>
+      <c r="H18" t="s">
+        <v>192</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[16] = new TableColDefEx("DoesNotRequirePreAuth", typeof(Boolean), "DONT_REQ_PREAUTH","UAC");</v>
+        <f>CONCATENATE("collist[",F18,"] = new TableColDefEx(""",C18,""", typeof(",B18,"), """,H18,""",""",G18,""");")</f>
+        <v>collist[16] = new TableColDefEx("Pager", typeof(String), "pager","Adprop");</v>
       </c>
       <c r="J18" t="str">
-        <f>CONCATENATE("[",C18,"] [",A18,"] ",E18,",")</f>
-        <v>[DoesNotRequirePreAuth] [bit] NULL,</v>
+        <f>CONCATENATE("[",C18,"] [",A18,"](",D18,") ",E18,",")</f>
+        <v>[Pager] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -7619,11 +7621,11 @@
       <c r="B19" t="s">
         <v>83</v>
       </c>
-      <c r="C19" t="s">
-        <v>23</v>
+      <c r="C19" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="D19">
-        <v>256</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
         <v>115</v>
@@ -7634,16 +7636,16 @@
       <c r="G19" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H19" s="15" t="s">
-        <v>123</v>
+      <c r="H19" t="s">
+        <v>95</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[17] = new TableColDefEx("EmailAddress", typeof(String), "mail","Adprop");</v>
+        <f>CONCATENATE("collist[",F19,"] = new TableColDefEx(""",C19,""", typeof(",B19,"), """,H19,""",""",G19,""");")</f>
+        <v>collist[17] = new TableColDefEx("MobilePhone", typeof(String), "mobile","Adprop");</v>
       </c>
       <c r="J19" t="str">
         <f>CONCATENATE("[",C19,"] [",A19,"](",D19,") ",E19,",")</f>
-        <v>[EmailAddress] [nvarchar](256) NULL,</v>
+        <v>[MobilePhone] [nvarchar](32) NULL,</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -7653,11 +7655,11 @@
       <c r="B20" t="s">
         <v>83</v>
       </c>
-      <c r="C20" t="s">
-        <v>24</v>
+      <c r="C20" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D20">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="E20" t="s">
         <v>115</v>
@@ -7668,16 +7670,16 @@
       <c r="G20" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H20" s="15" t="s">
-        <v>178</v>
+      <c r="H20" t="s">
+        <v>98</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[18] = new TableColDefEx("EmployeeID", typeof(String), "employeeid","Adprop");</v>
+        <f>CONCATENATE("collist[",F20,"] = new TableColDefEx(""",C20,""", typeof(",B20,"), """,H20,""",""",G20,""");")</f>
+        <v>collist[18] = new TableColDefEx("Fax", typeof(String), "facsimileTelephoneNumber","Adprop");</v>
       </c>
       <c r="J20" t="str">
         <f>CONCATENATE("[",C20,"] [",A20,"](",D20,") ",E20,",")</f>
-        <v>[EmployeeID] [nvarchar](64) NULL,</v>
+        <v>[Fax] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -7688,10 +7690,10 @@
         <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="D21">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="E21" t="s">
         <v>115</v>
@@ -7702,27 +7704,30 @@
       <c r="G21" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H21" s="15" t="s">
-        <v>188</v>
+      <c r="H21" t="s">
+        <v>175</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[19] = new TableColDefEx("EmployeeNumber", typeof(String), "employeenumber","Adprop");</v>
+        <f>CONCATENATE("collist[",F21,"] = new TableColDefEx(""",C21,""", typeof(",B21,"), """,H21,""",""",G21,""");")</f>
+        <v>collist[19] = new TableColDefEx("Title", typeof(String), "title","Adprop");</v>
       </c>
       <c r="J21" t="str">
         <f>CONCATENATE("[",C21,"] [",A21,"](",D21,") ",E21,",")</f>
-        <v>[EmployeeNumber] [nvarchar](64) NULL,</v>
+        <v>[Title] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="D22">
+        <v>128</v>
       </c>
       <c r="E22" t="s">
         <v>115</v>
@@ -7731,18 +7736,18 @@
         <v>20</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>161</v>
+        <v>173</v>
+      </c>
+      <c r="H22" t="s">
+        <v>185</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[20] = new TableColDefEx("Enabled", typeof(Boolean), "ACCOUNTDISABLE","UAC");</v>
+        <f>CONCATENATE("collist[",F22,"] = new TableColDefEx(""",C22,""", typeof(",B22,"), """,H22,""",""",G22,""");")</f>
+        <v>collist[20] = new TableColDefEx("Department", typeof(String), "department","Adprop");</v>
       </c>
       <c r="J22" t="str">
-        <f>CONCATENATE("[",C22,"] [",A22,"] ",E22,",")</f>
-        <v>[Enabled] [bit] NULL,</v>
+        <f>CONCATENATE("[",C22,"] [",A22,"](",D22,") ",E22,",")</f>
+        <v>[Department] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -7752,8 +7757,8 @@
       <c r="B23" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>27</v>
+      <c r="C23" t="s">
+        <v>14</v>
       </c>
       <c r="D23">
         <v>128</v>
@@ -7767,16 +7772,16 @@
       <c r="G23" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H23" s="15" t="s">
-        <v>98</v>
+      <c r="H23" t="s">
+        <v>180</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[21] = new TableColDefEx("Fax", typeof(String), "facsimileTelephoneNumber","Adprop");</v>
+        <f>CONCATENATE("collist[",F23,"] = new TableColDefEx(""",C23,""", typeof(",B23,"), """,H23,""",""",G23,""");")</f>
+        <v>collist[21] = new TableColDefEx("Company", typeof(String), "company","Adprop");</v>
       </c>
       <c r="J23" t="str">
         <f>CONCATENATE("[",C23,"] [",A23,"](",D23,") ",E23,",")</f>
-        <v>[Fax] [nvarchar](128) NULL,</v>
+        <v>[Company] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -7787,10 +7792,10 @@
         <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D24">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="E24" t="s">
         <v>115</v>
@@ -7801,16 +7806,16 @@
       <c r="G24" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H24" s="15" t="s">
-        <v>176</v>
+      <c r="H24" t="s">
+        <v>184</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[22] = new TableColDefEx("GivenName", typeof(String), "givenname","Adprop");</v>
+        <f>CONCATENATE("collist[",F24,"] = new TableColDefEx(""",C24,""", typeof(",B24,"), """,H24,""",""",G24,""");")</f>
+        <v>collist[22] = new TableColDefEx("Manager", typeof(String), "manager","Adprop");</v>
       </c>
       <c r="J24" t="str">
         <f>CONCATENATE("[",C24,"] [",A24,"](",D24,") ",E24,",")</f>
-        <v>[GivenName] [nvarchar](128) NULL,</v>
+        <v>[Manager] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -7820,11 +7825,11 @@
       <c r="B25" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>29</v>
+      <c r="C25" t="s">
+        <v>24</v>
       </c>
       <c r="D25">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
         <v>115</v>
@@ -7835,27 +7840,30 @@
       <c r="G25" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H25" s="15" t="s">
-        <v>189</v>
+      <c r="H25" t="s">
+        <v>178</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[23] = new TableColDefEx("HomeDirectory", typeof(String), "homedirectory","Adprop");</v>
+        <f>CONCATENATE("collist[",F25,"] = new TableColDefEx(""",C25,""", typeof(",B25,"), """,H25,""",""",G25,""");")</f>
+        <v>collist[23] = new TableColDefEx("EmployeeID", typeof(String), "employeeid","Adprop");</v>
       </c>
       <c r="J25" t="str">
         <f>CONCATENATE("[",C25,"] [",A25,"](",D25,") ",E25,",")</f>
-        <v>[HomeDirectory] [nvarchar](128) NULL,</v>
+        <v>[EmployeeID] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>30</v>
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>64</v>
       </c>
       <c r="E26" t="s">
         <v>115</v>
@@ -7864,18 +7872,18 @@
         <v>24</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H26" s="15" t="s">
-        <v>106</v>
+        <v>173</v>
+      </c>
+      <c r="H26" t="s">
+        <v>188</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[24] = new TableColDefEx("HomedirRequired", typeof(Boolean), "HOMEDIR_REQUIRED","UAC");</v>
+        <f>CONCATENATE("collist[",F26,"] = new TableColDefEx(""",C26,""", typeof(",B26,"), """,H26,""",""",G26,""");")</f>
+        <v>collist[24] = new TableColDefEx("EmployeeNumber", typeof(String), "employeenumber","Adprop");</v>
       </c>
       <c r="J26" t="str">
-        <f>CONCATENATE("[",C26,"] [",A26,"] ",E26,",")</f>
-        <v>[HomedirRequired] [bit] NULL,</v>
+        <f>CONCATENATE("[",C26,"] [",A26,"](",D26,") ",E26,",")</f>
+        <v>[EmployeeNumber] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -7885,11 +7893,11 @@
       <c r="B27" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>31</v>
+      <c r="C27" t="s">
+        <v>21</v>
       </c>
       <c r="D27">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="E27" t="s">
         <v>115</v>
@@ -7900,30 +7908,27 @@
       <c r="G27" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H27" s="15" t="s">
-        <v>190</v>
+      <c r="H27" t="s">
+        <v>187</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[25] = new TableColDefEx("HomeDrive", typeof(String), "homedrive","Adprop");</v>
+        <f>CONCATENATE("collist[",F27,"] = new TableColDefEx(""",C27,""", typeof(",B27,"), """,H27,""",""",G27,""");")</f>
+        <v>collist[25] = new TableColDefEx("Division", typeof(String), "division","Adprop");</v>
       </c>
       <c r="J27" t="str">
         <f>CONCATENATE("[",C27,"] [",A27,"](",D27,") ",E27,",")</f>
-        <v>[HomeDrive] [nvarchar](64) NULL,</v>
+        <v>[Division] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28">
-        <v>128</v>
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
       </c>
       <c r="E28" t="s">
         <v>115</v>
@@ -7932,32 +7937,29 @@
         <v>26</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H28" s="15" t="s">
-        <v>191</v>
+        <v>169</v>
+      </c>
+      <c r="H28" t="s">
+        <v>161</v>
       </c>
       <c r="I28" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[26] = new TableColDefEx("HomePage", typeof(String), "wwwhomepage","Adprop");</v>
+        <f>CONCATENATE("collist[",F28,"] = new TableColDefEx(""",C28,""", typeof(",B28,"), """,H28,""",""",G28,""");")</f>
+        <v>collist[26] = new TableColDefEx("Enabled", typeof(Boolean), "ACCOUNTDISABLE","UAC");</v>
       </c>
       <c r="J28" t="str">
-        <f>CONCATENATE("[",C28,"] [",A28,"](",D28,") ",E28,",")</f>
-        <v>[HomePage] [nvarchar](128) NULL,</v>
+        <f>CONCATENATE("[",C28,"] [",A28,"] ",E28,",")</f>
+        <v>[Enabled] [bit] NULL,</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29">
-        <v>32</v>
+        <v>80</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="E29" t="s">
         <v>115</v>
@@ -7966,32 +7968,29 @@
         <v>27</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>186</v>
+        <v>169</v>
+      </c>
+      <c r="H29" t="s">
+        <v>166</v>
       </c>
       <c r="I29" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[27] = new TableColDefEx("HomePhone", typeof(String), "homephone","Adprop");</v>
+        <f>CONCATENATE("collist[",F29,"] = new TableColDefEx(""",C29,""", typeof(",B29,"), """,H29,""",""",G29,""");")</f>
+        <v>collist[27] = new TableColDefEx("LockedOut", typeof(Boolean), "LOCKOUT","UAC");</v>
       </c>
       <c r="J29" t="str">
-        <f>CONCATENATE("[",C29,"] [",A29,"](",D29,") ",E29,",")</f>
-        <v>[HomePhone] [nvarchar](32) NULL,</v>
+        <f>CONCATENATE("[",C29,"] [",A29,"] ",E29,",")</f>
+        <v>[LockedOut] [bit] NULL,</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30">
-        <v>32</v>
+        <v>80</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="E30" t="s">
         <v>115</v>
@@ -8000,29 +7999,29 @@
         <v>28</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>182</v>
+        <v>169</v>
+      </c>
+      <c r="H30" t="s">
+        <v>103</v>
       </c>
       <c r="I30" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[28] = new TableColDefEx("Initials", typeof(String), "initials","Adprop");</v>
+        <f>CONCATENATE("collist[",F30,"] = new TableColDefEx(""",C30,""", typeof(",B30,"), """,H30,""",""",G30,""");")</f>
+        <v>collist[28] = new TableColDefEx("MNSLogonAccount", typeof(Boolean), "MNS_LOGON_ACCOUNT","UAC");</v>
       </c>
       <c r="J30" t="str">
-        <f>CONCATENATE("[",C30,"] [",A30,"](",D30,") ",E30,",")</f>
-        <v>[Initials] [nvarchar](32) NULL,</v>
+        <f>CONCATENATE("[",C30,"] [",A30,"] ",E30,",")</f>
+        <v>[MNSLogonAccount] [bit] NULL,</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="E31" t="s">
         <v>115</v>
@@ -8031,29 +8030,29 @@
         <v>29</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H31" s="19" t="s">
-        <v>156</v>
+        <v>169</v>
+      </c>
+      <c r="H31" t="s">
+        <v>163</v>
       </c>
       <c r="I31" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[29] = new TableColDefEx("LastBadPasswordAttempt", typeof(DateTime), "badpasswordtime","filetime");</v>
+        <f>CONCATENATE("collist[",F31,"] = new TableColDefEx(""",C31,""", typeof(",B31,"), """,H31,""",""",G31,""");")</f>
+        <v>collist[29] = new TableColDefEx("CannotChangePassword", typeof(Boolean), "PASSWD_CANT_CHANGE","UAC");</v>
       </c>
       <c r="J31" t="str">
         <f>CONCATENATE("[",C31,"] [",A31,"] ",E31,",")</f>
-        <v>[LastBadPasswordAttempt] [datetime] NULL,</v>
+        <v>[CannotChangePassword] [bit] NULL,</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" t="s">
-        <v>36</v>
+        <v>80</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="E32" t="s">
         <v>115</v>
@@ -8062,18 +8061,18 @@
         <v>30</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H32" s="19" t="s">
-        <v>199</v>
+        <v>169</v>
+      </c>
+      <c r="H32" t="s">
+        <v>104</v>
       </c>
       <c r="I32" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[30] = new TableColDefEx("LastLogonDate", typeof(DateTime), "lastlogon","filetime");</v>
+        <f>CONCATENATE("collist[",F32,"] = new TableColDefEx(""",C32,""", typeof(",B32,"), """,H32,""",""",G32,""");")</f>
+        <v>collist[30] = new TableColDefEx("PasswordExpired", typeof(Boolean), "PASSWORD_EXPIRED","UAC");</v>
       </c>
       <c r="J32" t="str">
         <f>CONCATENATE("[",C32,"] [",A32,"] ",E32,",")</f>
-        <v>[LastLogonDate] [datetime] NULL,</v>
+        <v>[PasswordExpired] [bit] NULL,</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -8083,8 +8082,8 @@
       <c r="B33" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>37</v>
+      <c r="C33" t="s">
+        <v>52</v>
       </c>
       <c r="E33" t="s">
         <v>115</v>
@@ -8095,27 +8094,27 @@
       <c r="G33" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H33" s="15" t="s">
-        <v>166</v>
+      <c r="H33" t="s">
+        <v>164</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[31] = new TableColDefEx("LockedOut", typeof(Boolean), "LOCKOUT","UAC");</v>
+        <f>CONCATENATE("collist[",F33,"] = new TableColDefEx(""",C33,""", typeof(",B33,"), """,H33,""",""",G33,""");")</f>
+        <v>collist[31] = new TableColDefEx("PasswordNeverExpires", typeof(Boolean), "DONT_EXPIRE_PASSWD","UAC");</v>
       </c>
       <c r="J33" t="str">
         <f>CONCATENATE("[",C33,"] [",A33,"] ",E33,",")</f>
-        <v>[LockedOut] [bit] NULL,</v>
+        <v>[PasswordNeverExpires] [bit] NULL,</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>200</v>
+        <v>80</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
       </c>
       <c r="E34" t="s">
         <v>115</v>
@@ -8124,32 +8123,29 @@
         <v>32</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H34" s="18" t="s">
-        <v>147</v>
+        <v>169</v>
+      </c>
+      <c r="H34" t="s">
+        <v>162</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[32] = new TableColDefEx("LogonCount", typeof(Int32), "logoncount","Adprop");</v>
+        <f>CONCATENATE("collist[",F34,"] = new TableColDefEx(""",C34,""", typeof(",B34,"), """,H34,""",""",G34,""");")</f>
+        <v>collist[32] = new TableColDefEx("PasswordNotRequired", typeof(Boolean), "PASSWD_NOTREQD","UAC");</v>
       </c>
       <c r="J34" t="str">
         <f>CONCATENATE("[",C34,"] [",A34,"] ",E34,",")</f>
-        <v>[LogonCount] [int] NULL,</v>
+        <v>[PasswordNotRequired] [bit] NULL,</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35">
-        <v>128</v>
+        <v>80</v>
+      </c>
+      <c r="C35" t="s">
+        <v>60</v>
       </c>
       <c r="E35" t="s">
         <v>115</v>
@@ -8158,32 +8154,29 @@
         <v>33</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H35" s="15" t="s">
-        <v>198</v>
+        <v>169</v>
+      </c>
+      <c r="H35" t="s">
+        <v>165</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[33] = new TableColDefEx("LogonWorkstations", typeof(String), "userworkstations","Adprop");</v>
+        <f>CONCATENATE("collist[",F35,"] = new TableColDefEx(""",C35,""", typeof(",B35,"), """,H35,""",""",G35,""");")</f>
+        <v>collist[33] = new TableColDefEx("SmartcardLogonRequired", typeof(Boolean), "SMARTCARD_REQUIRED","UAC");</v>
       </c>
       <c r="J35" t="str">
-        <f>CONCATENATE("[",C35,"] [",A35,"](",D35,") ",E35,",")</f>
-        <v>[LogonWorkstations] [nvarchar](128) NULL,</v>
+        <f>CONCATENATE("[",C35,"] [",A35,"] ",E35,",")</f>
+        <v>[SmartcardLogonRequired] [bit] NULL,</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36">
-        <v>256</v>
+        <v>80</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="E36" t="s">
         <v>115</v>
@@ -8192,18 +8185,18 @@
         <v>34</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H36" s="15" t="s">
-        <v>184</v>
+        <v>169</v>
+      </c>
+      <c r="H36" t="s">
+        <v>107</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[34] = new TableColDefEx("Manager", typeof(String), "manager","Adprop");</v>
+        <f>CONCATENATE("collist[",F36,"] = new TableColDefEx(""",C36,""", typeof(",B36,"), """,H36,""",""",G36,""");")</f>
+        <v>collist[34] = new TableColDefEx("DoesNotRequirePreAuth", typeof(Boolean), "DONT_REQ_PREAUTH","UAC");</v>
       </c>
       <c r="J36" t="str">
-        <f>CONCATENATE("[",C36,"] [",A36,"](",D36,") ",E36,",")</f>
-        <v>[Manager] [nvarchar](256) NULL,</v>
+        <f>CONCATENATE("[",C36,"] [",A36,"] ",E36,",")</f>
+        <v>[DoesNotRequirePreAuth] [bit] NULL,</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -8213,8 +8206,8 @@
       <c r="B37" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="12" t="s">
-        <v>40</v>
+      <c r="C37" t="s">
+        <v>7</v>
       </c>
       <c r="E37" t="s">
         <v>115</v>
@@ -8225,30 +8218,27 @@
       <c r="G37" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H37" s="15" t="s">
-        <v>103</v>
+      <c r="H37" t="s">
+        <v>167</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[35] = new TableColDefEx("MNSLogonAccount", typeof(Boolean), "MNS_LOGON_ACCOUNT","UAC");</v>
+        <f>CONCATENATE("collist[",F37,"] = new TableColDefEx(""",C37,""", typeof(",B37,"), """,H37,""",""",G37,""");")</f>
+        <v>collist[35] = new TableColDefEx("AllowReversiblePasswordEncryption", typeof(Boolean), "ENCRYPTED_TEXT_PWD_ALLOWED","UAC");</v>
       </c>
       <c r="J37" t="str">
         <f>CONCATENATE("[",C37,"] [",A37,"] ",E37,",")</f>
-        <v>[MNSLogonAccount] [bit] NULL,</v>
+        <v>[AllowReversiblePasswordEncryption] [bit] NULL,</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="E38" t="s">
         <v>115</v>
@@ -8257,29 +8247,29 @@
         <v>36</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>95</v>
+        <v>169</v>
+      </c>
+      <c r="H38" t="s">
+        <v>105</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[36] = new TableColDefEx("MobilePhone", typeof(String), "mobile","Adprop");</v>
+        <f>CONCATENATE("collist[",F38,"] = new TableColDefEx(""",C38,""", typeof(",B38,"), """,H38,""",""",G38,""");")</f>
+        <v>collist[36] = new TableColDefEx("AccountNotDelegated", typeof(Boolean), "NOT_DELEGATED","UAC");</v>
       </c>
       <c r="J38" t="str">
-        <f>CONCATENATE("[",C38,"] [",A38,"](",D38,") ",E38,",")</f>
-        <v>[MobilePhone] [nvarchar](32) NULL,</v>
+        <f>CONCATENATE("[",C38,"] [",A38,"] ",E38,",")</f>
+        <v>[AccountNotDelegated] [bit] NULL,</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="E39" t="s">
         <v>115</v>
@@ -8288,32 +8278,29 @@
         <v>37</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>177</v>
+        <v>169</v>
+      </c>
+      <c r="H39" t="s">
+        <v>102</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[37] = new TableColDefEx("Modified", typeof(DateTime), "whenchanged","Adprop");</v>
+        <f>CONCATENATE("collist[",F39,"] = new TableColDefEx(""",C39,""", typeof(",B39,"), """,H39,""",""",G39,""");")</f>
+        <v>collist[37] = new TableColDefEx("TrustedForDelegation", typeof(Boolean), "TRUSTED_FOR_DELEGATION","UAC");</v>
       </c>
       <c r="J39" t="str">
-        <f>CONCATENATE("[",C39,"] [",A39,"] ",E39,",")</f>
-        <v>[Modified] [datetime] NULL,</v>
+        <f t="shared" ref="J39:J41" si="0">CONCATENATE("[",C39,"] [",A39,"] ",E39,",")</f>
+        <v>[TrustedForDelegation] [bit] NULL,</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40">
-        <v>256</v>
+        <v>80</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="E40" t="s">
         <v>115</v>
@@ -8322,32 +8309,29 @@
         <v>38</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H40" s="15" t="s">
-        <v>127</v>
+        <v>169</v>
+      </c>
+      <c r="H40" t="s">
+        <v>100</v>
       </c>
       <c r="I40" s="1" t="str">
+        <f>CONCATENATE("collist[",F40,"] = new TableColDefEx(""",C40,""", typeof(",B40,"), """,H40,""",""",G40,""");")</f>
+        <v>collist[38] = new TableColDefEx("TrustedToAuthForDelegation", typeof(Boolean), "TRUSTED_TO_AUTH_FOR_DELEGATION","UAC");</v>
+      </c>
+      <c r="J40" t="str">
         <f t="shared" si="0"/>
-        <v>collist[38] = new TableColDefEx("Name", typeof(String), "name","Adprop");</v>
-      </c>
-      <c r="J40" t="str">
-        <f>CONCATENATE("[",C40,"] [",A40,"](",D40,") ",E40,",")</f>
-        <v>[Name] [nvarchar](256) NULL,</v>
+        <v>[TrustedToAuthForDelegation] [bit] NULL,</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41">
-        <v>128</v>
+        <v>80</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="E41" t="s">
         <v>115</v>
@@ -8356,32 +8340,29 @@
         <v>39</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H41" s="15" t="s">
-        <v>139</v>
+        <v>169</v>
+      </c>
+      <c r="H41" t="s">
+        <v>101</v>
       </c>
       <c r="I41" s="1" t="str">
+        <f>CONCATENATE("collist[",F41,"] = new TableColDefEx(""",C41,""", typeof(",B41,"), """,H41,""",""",G41,""");")</f>
+        <v>collist[39] = new TableColDefEx("UseDESKeyOnly", typeof(Boolean), "USE_DES_KEY_ONLY","UAC");</v>
+      </c>
+      <c r="J41" t="str">
         <f t="shared" si="0"/>
-        <v>collist[39] = new TableColDefEx("ObjectCategory", typeof(String), "objectcategory","Adprop");</v>
-      </c>
-      <c r="J41" t="str">
-        <f>CONCATENATE("[",C41,"] [",A41,"](",D41,") ",E41,",")</f>
-        <v>[ObjectCategory] [nvarchar](128) NULL,</v>
+        <v>[UseDESKeyOnly] [bit] NULL,</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42">
-        <v>64</v>
+        <v>80</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="E42" t="s">
         <v>115</v>
@@ -8390,63 +8371,60 @@
         <v>40</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>144</v>
+        <v>169</v>
+      </c>
+      <c r="H42" t="s">
+        <v>106</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[40] = new TableColDefEx("ObjectClass", typeof(String), "SchemaClassName","ObjClass");</v>
+        <f>CONCATENATE("collist[",F42,"] = new TableColDefEx(""",C42,""", typeof(",B42,"), """,H42,""",""",G42,""");")</f>
+        <v>collist[40] = new TableColDefEx("HomedirRequired", typeof(Boolean), "HOMEDIR_REQUIRED","UAC");</v>
       </c>
       <c r="J42" t="str">
-        <f>CONCATENATE("[",C42,"] [",A42,"](",D42,") ",E42,",")</f>
-        <v>[ObjectClass] [nvarchar](64) NULL,</v>
+        <f>CONCATENATE("[",C42,"] [",A42,"] ",E42,",")</f>
+        <v>[HomedirRequired] [bit] NULL,</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C43" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F43" s="6">
         <v>41</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>71</v>
+        <v>170</v>
+      </c>
+      <c r="H43" t="s">
+        <v>156</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[41] = new TableColDefEx("ObjectGUID", typeof(Guid), "Guid","ObjGuid");</v>
+        <f>CONCATENATE("collist[",F43,"] = new TableColDefEx(""",C43,""", typeof(",B43,"), """,H43,""",""",G43,""");")</f>
+        <v>collist[41] = new TableColDefEx("LastBadPasswordAttempt", typeof(DateTime), "badpasswordtime","filetime");</v>
       </c>
       <c r="J43" t="str">
         <f>CONCATENATE("[",C43,"] [",A43,"] ",E43,",")</f>
-        <v>[ObjectGUID] [uniqueidentifier] NOT NULL,</v>
+        <v>[LastBadPasswordAttempt] [datetime] NULL,</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44">
-        <v>128</v>
+        <v>82</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
       </c>
       <c r="E44" t="s">
         <v>115</v>
@@ -8457,30 +8435,27 @@
       <c r="G44" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H44" s="15" t="s">
-        <v>91</v>
+      <c r="H44" t="s">
+        <v>150</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[42] = new TableColDefEx("Office", typeof(String), "physicalDeliveryOfficeName","Adprop");</v>
+        <f>CONCATENATE("collist[",F44,"] = new TableColDefEx(""",C44,""", typeof(",B44,"), """,H44,""",""",G44,""");")</f>
+        <v>collist[42] = new TableColDefEx("BadLogonCount", typeof(Int32), "badpwdcount","Adprop");</v>
       </c>
       <c r="J44" t="str">
-        <f>CONCATENATE("[",C44,"] [",A44,"](",D44,") ",E44,",")</f>
-        <v>[Office] [nvarchar](128) NULL,</v>
+        <f>CONCATENATE("[",C44,"] [",A44,"] ",E44,",")</f>
+        <v>[BadLogonCount] [int] NULL,</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45">
-        <v>32</v>
+        <v>81</v>
+      </c>
+      <c r="C45" t="s">
+        <v>36</v>
       </c>
       <c r="E45" t="s">
         <v>115</v>
@@ -8489,32 +8464,29 @@
         <v>43</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H45" s="15" t="s">
-        <v>181</v>
+        <v>170</v>
+      </c>
+      <c r="H45" t="s">
+        <v>199</v>
       </c>
       <c r="I45" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[43] = new TableColDefEx("OfficePhone", typeof(String), "telephonenumber","Adprop");</v>
+        <f>CONCATENATE("collist[",F45,"] = new TableColDefEx(""",C45,""", typeof(",B45,"), """,H45,""",""",G45,""");")</f>
+        <v>collist[43] = new TableColDefEx("LastLogonDate", typeof(DateTime), "lastlogon","filetime");</v>
       </c>
       <c r="J45" t="str">
-        <f>CONCATENATE("[",C45,"] [",A45,"](",D45,") ",E45,",")</f>
-        <v>[OfficePhone] [nvarchar](32) NULL,</v>
+        <f>CONCATENATE("[",C45,"] [",A45,"] ",E45,",")</f>
+        <v>[LastLogonDate] [datetime] NULL,</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" t="s">
-        <v>69</v>
-      </c>
-      <c r="D46">
-        <v>32</v>
+        <v>82</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>200</v>
       </c>
       <c r="E46" t="s">
         <v>115</v>
@@ -8525,27 +8497,27 @@
       <c r="G46" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H46" s="15" t="s">
-        <v>192</v>
+      <c r="H46" t="s">
+        <v>147</v>
       </c>
       <c r="I46" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[44] = new TableColDefEx("Pager", typeof(String), "pager","Adprop");</v>
+        <f>CONCATENATE("collist[",F46,"] = new TableColDefEx(""",C46,""", typeof(",B46,"), """,H46,""",""",G46,""");")</f>
+        <v>collist[44] = new TableColDefEx("LogonCount", typeof(Int32), "logoncount","Adprop");</v>
       </c>
       <c r="J46" t="str">
-        <f>CONCATENATE("[",C46,"] [",A46,"](",D46,") ",E46,",")</f>
-        <v>[Pager] [nvarchar](32) NULL,</v>
+        <f>CONCATENATE("[",C46,"] [",A46,"] ",E46,",")</f>
+        <v>[LogonCount] [int] NULL,</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>50</v>
+        <v>81</v>
+      </c>
+      <c r="C47" t="s">
+        <v>51</v>
       </c>
       <c r="E47" t="s">
         <v>115</v>
@@ -8554,18 +8526,18 @@
         <v>45</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>104</v>
+        <v>170</v>
+      </c>
+      <c r="H47" t="s">
+        <v>149</v>
       </c>
       <c r="I47" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[45] = new TableColDefEx("PasswordExpired", typeof(Boolean), "PASSWORD_EXPIRED","UAC");</v>
+        <f>CONCATENATE("collist[",F47,"] = new TableColDefEx(""",C47,""", typeof(",B47,"), """,H47,""",""",G47,""");")</f>
+        <v>collist[45] = new TableColDefEx("PasswordLastSet", typeof(DateTime), "pwdlastset","filetime");</v>
       </c>
       <c r="J47" t="str">
         <f>CONCATENATE("[",C47,"] [",A47,"] ",E47,",")</f>
-        <v>[PasswordExpired] [bit] NULL,</v>
+        <v>[PasswordLastSet] [datetime] NULL,</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -8576,7 +8548,7 @@
         <v>81</v>
       </c>
       <c r="C48" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="E48" t="s">
         <v>115</v>
@@ -8587,27 +8559,27 @@
       <c r="G48" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H48" s="19" t="s">
-        <v>149</v>
+      <c r="H48" t="s">
+        <v>168</v>
       </c>
       <c r="I48" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[46] = new TableColDefEx("PasswordLastSet", typeof(DateTime), "pwdlastset","filetime");</v>
+        <f>CONCATENATE("collist[",F48,"] = new TableColDefEx(""",C48,""", typeof(",B48,"), """,H48,""",""",G48,""");")</f>
+        <v>collist[46] = new TableColDefEx("AccountLockoutTime", typeof(DateTime), "lockouttime","filetime");</v>
       </c>
       <c r="J48" t="str">
         <f>CONCATENATE("[",C48,"] [",A48,"] ",E48,",")</f>
-        <v>[PasswordLastSet] [datetime] NULL,</v>
+        <v>[AccountLockoutTime] [datetime] NULL,</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="E49" t="s">
         <v>115</v>
@@ -8616,29 +8588,32 @@
         <v>47</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H49" s="15" t="s">
-        <v>164</v>
+        <v>170</v>
+      </c>
+      <c r="H49" t="s">
+        <v>145</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[47] = new TableColDefEx("PasswordNeverExpires", typeof(Boolean), "DONT_EXPIRE_PASSWD","UAC");</v>
+        <f>CONCATENATE("collist[",F49,"] = new TableColDefEx(""",C49,""", typeof(",B49,"), """,H49,""",""",G49,""");")</f>
+        <v>collist[47] = new TableColDefEx("AccountExpirationDate", typeof(DateTime), "accountexpires","filetime");</v>
       </c>
       <c r="J49" t="str">
         <f>CONCATENATE("[",C49,"] [",A49,"] ",E49,",")</f>
-        <v>[PasswordNeverExpires] [bit] NULL,</v>
+        <v>[AccountExpirationDate] [datetime] NULL,</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
-      </c>
-      <c r="C50" t="s">
-        <v>53</v>
+        <v>83</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50">
+        <v>128</v>
       </c>
       <c r="E50" t="s">
         <v>115</v>
@@ -8647,18 +8622,18 @@
         <v>48</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H50" s="15" t="s">
-        <v>162</v>
+        <v>173</v>
+      </c>
+      <c r="H50" t="s">
+        <v>198</v>
       </c>
       <c r="I50" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[48] = new TableColDefEx("PasswordNotRequired", typeof(Boolean), "PASSWD_NOTREQD","UAC");</v>
+        <f>CONCATENATE("collist[",F50,"] = new TableColDefEx(""",C50,""", typeof(",B50,"), """,H50,""",""",G50,""");")</f>
+        <v>collist[48] = new TableColDefEx("LogonWorkstations", typeof(String), "userworkstations","Adprop");</v>
       </c>
       <c r="J50" t="str">
-        <f>CONCATENATE("[",C50,"] [",A50,"] ",E50,",")</f>
-        <v>[PasswordNotRequired] [bit] NULL,</v>
+        <f>CONCATENATE("[",C50,"] [",A50,"](",D50,") ",E50,",")</f>
+        <v>[LogonWorkstations] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -8669,10 +8644,10 @@
         <v>83</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D51">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="E51" t="s">
         <v>115</v>
@@ -8683,16 +8658,16 @@
       <c r="G51" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H51" s="15" t="s">
-        <v>193</v>
+      <c r="H51" t="s">
+        <v>189</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[49] = new TableColDefEx("POBox", typeof(String), "postofficebox","Adprop");</v>
+        <f>CONCATENATE("collist[",F51,"] = new TableColDefEx(""",C51,""", typeof(",B51,"), """,H51,""",""",G51,""");")</f>
+        <v>collist[49] = new TableColDefEx("HomeDirectory", typeof(String), "homedirectory","Adprop");</v>
       </c>
       <c r="J51" t="str">
         <f>CONCATENATE("[",C51,"] [",A51,"](",D51,") ",E51,",")</f>
-        <v>[POBox] [nvarchar](32) NULL,</v>
+        <v>[HomeDirectory] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -8702,11 +8677,11 @@
       <c r="B52" t="s">
         <v>83</v>
       </c>
-      <c r="C52" t="s">
-        <v>55</v>
+      <c r="C52" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="D52">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="E52" t="s">
         <v>115</v>
@@ -8717,27 +8692,27 @@
       <c r="G52" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H52" s="15" t="s">
-        <v>194</v>
+      <c r="H52" t="s">
+        <v>190</v>
       </c>
       <c r="I52" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[50] = new TableColDefEx("PostalCode", typeof(String), "postalcode","Adprop");</v>
+        <f>CONCATENATE("collist[",F52,"] = new TableColDefEx(""",C52,""", typeof(",B52,"), """,H52,""",""",G52,""");")</f>
+        <v>collist[50] = new TableColDefEx("HomeDrive", typeof(String), "homedrive","Adprop");</v>
       </c>
       <c r="J52" t="str">
         <f>CONCATENATE("[",C52,"] [",A52,"](",D52,") ",E52,",")</f>
-        <v>[PostalCode] [nvarchar](32) NULL,</v>
+        <v>[HomeDrive] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>109</v>
+        <v>83</v>
+      </c>
+      <c r="C53" t="s">
+        <v>56</v>
       </c>
       <c r="D53">
         <v>128</v>
@@ -8751,16 +8726,16 @@
       <c r="G53" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H53" s="15" t="s">
-        <v>153</v>
+      <c r="H53" t="s">
+        <v>195</v>
       </c>
       <c r="I53" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[51] = new TableColDefEx("PrimaryGroupID", typeof(Int32), "primarygroupid","Adprop");</v>
+        <f t="shared" ref="I53:I54" si="1">CONCATENATE("collist[",F53,"] = new TableColDefEx(""",C53,""", typeof(",B53,"), """,H53,""",""",G53,""");")</f>
+        <v>collist[51] = new TableColDefEx("ProfilePath", typeof(String), "profilepath","Adprop");</v>
       </c>
       <c r="J53" t="str">
-        <f>CONCATENATE("[",C53,"] [",A53,"] ",E53,",")</f>
-        <v>[PrimaryGroupID] [int] NULL,</v>
+        <f>CONCATENATE("[",C53,"] [",A53,"](",D53,") ",E53,",")</f>
+        <v>[ProfilePath] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -8771,10 +8746,10 @@
         <v>83</v>
       </c>
       <c r="C54" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D54">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="E54" t="s">
         <v>115</v>
@@ -8785,30 +8760,27 @@
       <c r="G54" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H54" s="15" t="s">
-        <v>195</v>
+      <c r="H54" t="s">
+        <v>196</v>
       </c>
       <c r="I54" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[52] = new TableColDefEx("ProfilePath", typeof(String), "profilepath","Adprop");</v>
+        <f t="shared" si="1"/>
+        <v>collist[52] = new TableColDefEx("ScriptPath", typeof(String), "scriptpath","Adprop");</v>
       </c>
       <c r="J54" t="str">
         <f>CONCATENATE("[",C54,"] [",A54,"](",D54,") ",E54,",")</f>
-        <v>[ProfilePath] [nvarchar](128) NULL,</v>
+        <v>[ScriptPath] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C55" t="s">
-        <v>57</v>
-      </c>
-      <c r="D55">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="E55" t="s">
         <v>115</v>
@@ -8819,30 +8791,30 @@
       <c r="G55" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H55" s="15" t="s">
-        <v>137</v>
+      <c r="H55" t="s">
+        <v>146</v>
       </c>
       <c r="I55" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[53] = new TableColDefEx("SamAccountName", typeof(String), "samaccountname","Adprop");</v>
+        <f t="shared" ref="I55" si="2">CONCATENATE("collist[",F55,"] = new TableColDefEx(""",C55,""", typeof(",B55,"), """,H55,""",""",G55,""");")</f>
+        <v>collist[53] = new TableColDefEx("userAccountControl", typeof(Int32), "useraccountcontrol","Adprop");</v>
       </c>
       <c r="J55" t="str">
-        <f>CONCATENATE("[",C55,"] [",A55,"](",D55,") ",E55,",")</f>
-        <v>[SamAccountName] [nvarchar](128) NULL,</v>
+        <f>CONCATENATE("[",C55,"] [",A55,"] ",E55,",")</f>
+        <v>[userAccountControl] [int] NULL,</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
-      </c>
-      <c r="C56" t="s">
-        <v>58</v>
+        <v>82</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="D56">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="E56" t="s">
         <v>115</v>
@@ -8853,16 +8825,16 @@
       <c r="G56" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H56" s="15" t="s">
-        <v>196</v>
+      <c r="H56" t="s">
+        <v>153</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[54] = new TableColDefEx("ScriptPath", typeof(String), "scriptpath","Adprop");</v>
+        <f>CONCATENATE("collist[",F56,"] = new TableColDefEx(""",C56,""", typeof(",B56,"), """,H56,""",""",G56,""");")</f>
+        <v>collist[54] = new TableColDefEx("PrimaryGroupID", typeof(Int32), "primarygroupid","Adprop");</v>
       </c>
       <c r="J56" t="str">
-        <f>CONCATENATE("[",C56,"] [",A56,"](",D56,") ",E56,",")</f>
-        <v>[ScriptPath] [nvarchar](256) NULL,</v>
+        <f>CONCATENATE("[",C56,"] [",A56,"] ",E56,",")</f>
+        <v>[PrimaryGroupID] [int] NULL,</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -8873,41 +8845,44 @@
         <v>83</v>
       </c>
       <c r="C57" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D57">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="E57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F57" s="6">
         <v>55</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H57" s="15" t="s">
-        <v>138</v>
+        <v>173</v>
+      </c>
+      <c r="H57" t="s">
+        <v>127</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[55] = new TableColDefEx("SID", typeof(String), "objectsid","SID");</v>
+        <f>CONCATENATE("collist[",F57,"] = new TableColDefEx(""",C57,""", typeof(",B57,"), """,H57,""",""",G57,""");")</f>
+        <v>collist[55] = new TableColDefEx("Name", typeof(String), "name","Adprop");</v>
       </c>
       <c r="J57" t="str">
         <f>CONCATENATE("[",C57,"] [",A57,"](",D57,") ",E57,",")</f>
-        <v>[SID] [nvarchar](128) NOT NULL,</v>
+        <v>[Name] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C58" t="s">
-        <v>60</v>
+        <v>13</v>
+      </c>
+      <c r="D58">
+        <v>256</v>
       </c>
       <c r="E58" t="s">
         <v>115</v>
@@ -8916,18 +8891,18 @@
         <v>56</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H58" s="15" t="s">
-        <v>165</v>
+        <v>173</v>
+      </c>
+      <c r="H58" t="s">
+        <v>152</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[56] = new TableColDefEx("SmartcardLogonRequired", typeof(Boolean), "SMARTCARD_REQUIRED","UAC");</v>
+        <f>CONCATENATE("collist[",F58,"] = new TableColDefEx(""",C58,""", typeof(",B58,"), """,H58,""",""",G58,""");")</f>
+        <v>collist[56] = new TableColDefEx("CN", typeof(String), "cn","Adprop");</v>
       </c>
       <c r="J58" t="str">
-        <f>CONCATENATE("[",C58,"] [",A58,"] ",E58,",")</f>
-        <v>[SmartcardLogonRequired] [bit] NULL,</v>
+        <f>CONCATENATE("[",C58,"] [",A58,"](",D58,") ",E58,",")</f>
+        <v>[CN] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -8937,11 +8912,11 @@
       <c r="B59" t="s">
         <v>83</v>
       </c>
-      <c r="C59" s="12" t="s">
-        <v>61</v>
+      <c r="C59" t="s">
+        <v>68</v>
       </c>
       <c r="D59">
-        <v>64</v>
+        <v>256</v>
       </c>
       <c r="E59" t="s">
         <v>115</v>
@@ -8952,16 +8927,16 @@
       <c r="G59" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H59" s="15" t="s">
-        <v>90</v>
+      <c r="H59" t="s">
+        <v>179</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[57] = new TableColDefEx("State", typeof(String), "st","Adprop");</v>
+        <f>CONCATENATE("collist[",F59,"] = new TableColDefEx(""",C59,""", typeof(",B59,"), """,H59,""",""",G59,""");")</f>
+        <v>collist[57] = new TableColDefEx("UserPrincipalName", typeof(String), "userprincipalname","Adprop");</v>
       </c>
       <c r="J59" t="str">
         <f>CONCATENATE("[",C59,"] [",A59,"](",D59,") ",E59,",")</f>
-        <v>[State] [nvarchar](64) NULL,</v>
+        <v>[UserPrincipalName] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -8972,10 +8947,10 @@
         <v>83</v>
       </c>
       <c r="C60" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D60">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="E60" t="s">
         <v>115</v>
@@ -8986,16 +8961,16 @@
       <c r="G60" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H60" s="15" t="s">
-        <v>197</v>
+      <c r="H60" t="s">
+        <v>137</v>
       </c>
       <c r="I60" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[58] = new TableColDefEx("StreetAddress", typeof(String), "streetaddress","Adprop");</v>
+        <f>CONCATENATE("collist[",F60,"] = new TableColDefEx(""",C60,""", typeof(",B60,"), """,H60,""",""",G60,""");")</f>
+        <v>collist[58] = new TableColDefEx("SamAccountName", typeof(String), "samaccountname","Adprop");</v>
       </c>
       <c r="J60" t="str">
         <f>CONCATENATE("[",C60,"] [",A60,"](",D60,") ",E60,",")</f>
-        <v>[StreetAddress] [nvarchar](160) NULL,</v>
+        <v>[SamAccountName] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -9006,10 +8981,10 @@
         <v>83</v>
       </c>
       <c r="C61" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="D61">
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="E61" t="s">
         <v>115</v>
@@ -9020,30 +8995,27 @@
       <c r="G61" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H61" s="15" t="s">
-        <v>126</v>
+      <c r="H61" t="s">
+        <v>140</v>
       </c>
       <c r="I61" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[59] = new TableColDefEx("Surname", typeof(String), "sn","Adprop");</v>
+        <f>CONCATENATE("collist[",F61,"] = new TableColDefEx(""",C61,""", typeof(",B61,"), """,H61,""",""",G61,""");")</f>
+        <v>collist[59] = new TableColDefEx("DistinguishedName", typeof(String), "distinguishedname","Adprop");</v>
       </c>
       <c r="J61" t="str">
         <f>CONCATENATE("[",C61,"] [",A61,"](",D61,") ",E61,",")</f>
-        <v>[Surname] [nvarchar](256) NULL,</v>
+        <v>[DistinguishedName] [nvarchar](512) NULL,</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>83</v>
-      </c>
-      <c r="C62" t="s">
-        <v>64</v>
-      </c>
-      <c r="D62">
-        <v>128</v>
+        <v>81</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="E62" t="s">
         <v>115</v>
@@ -9054,27 +9026,27 @@
       <c r="G62" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H62" s="15" t="s">
-        <v>175</v>
+      <c r="H62" t="s">
+        <v>183</v>
       </c>
       <c r="I62" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[60] = new TableColDefEx("Title", typeof(String), "title","Adprop");</v>
+        <f>CONCATENATE("collist[",F62,"] = new TableColDefEx(""",C62,""", typeof(",B62,"), """,H62,""",""",G62,""");")</f>
+        <v>collist[60] = new TableColDefEx("Created", typeof(DateTime), "whencreated","Adprop");</v>
       </c>
       <c r="J62" t="str">
-        <f>CONCATENATE("[",C62,"] [",A62,"](",D62,") ",E62,",")</f>
-        <v>[Title] [nvarchar](128) NULL,</v>
+        <f>CONCATENATE("[",C62,"] [",A62,"] ",E62,",")</f>
+        <v>[Created] [datetime] NULL,</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="E63" t="s">
         <v>115</v>
@@ -9083,29 +9055,32 @@
         <v>61</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H63" s="15" t="s">
-        <v>102</v>
+        <v>173</v>
+      </c>
+      <c r="H63" t="s">
+        <v>177</v>
       </c>
       <c r="I63" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[61] = new TableColDefEx("TrustedForDelegation", typeof(Boolean), "TRUSTED_FOR_DELEGATION","UAC");</v>
+        <f>CONCATENATE("collist[",F63,"] = new TableColDefEx(""",C63,""", typeof(",B63,"), """,H63,""",""",G63,""");")</f>
+        <v>collist[61] = new TableColDefEx("Modified", typeof(DateTime), "whenchanged","Adprop");</v>
       </c>
       <c r="J63" t="str">
-        <f t="shared" ref="J63:J67" si="1">CONCATENATE("[",C63,"] [",A63,"] ",E63,",")</f>
-        <v>[TrustedForDelegation] [bit] NULL,</v>
+        <f>CONCATENATE("[",C63,"] [",A63,"] ",E63,",")</f>
+        <v>[Modified] [datetime] NULL,</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>80</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>66</v>
+        <v>83</v>
+      </c>
+      <c r="C64" t="s">
+        <v>44</v>
+      </c>
+      <c r="D64">
+        <v>128</v>
       </c>
       <c r="E64" t="s">
         <v>115</v>
@@ -9114,29 +9089,32 @@
         <v>62</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H64" s="15" t="s">
-        <v>100</v>
+        <v>173</v>
+      </c>
+      <c r="H64" t="s">
+        <v>139</v>
       </c>
       <c r="I64" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[62] = new TableColDefEx("TrustedToAuthForDelegation", typeof(Boolean), "TRUSTED_TO_AUTH_FOR_DELEGATION","UAC");</v>
+        <f>CONCATENATE("collist[",F64,"] = new TableColDefEx(""",C64,""", typeof(",B64,"), """,H64,""",""",G64,""");")</f>
+        <v>collist[62] = new TableColDefEx("ObjectCategory", typeof(String), "objectcategory","Adprop");</v>
       </c>
       <c r="J64" t="str">
-        <f t="shared" si="1"/>
-        <v>[TrustedToAuthForDelegation] [bit] NULL,</v>
+        <f>CONCATENATE("[",C64,"] [",A64,"](",D64,") ",E64,",")</f>
+        <v>[ObjectCategory] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>67</v>
+        <v>83</v>
+      </c>
+      <c r="C65" t="s">
+        <v>45</v>
+      </c>
+      <c r="D65">
+        <v>64</v>
       </c>
       <c r="E65" t="s">
         <v>115</v>
@@ -9145,18 +9123,18 @@
         <v>63</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H65" s="15" t="s">
-        <v>101</v>
+        <v>171</v>
+      </c>
+      <c r="H65" t="s">
+        <v>144</v>
       </c>
       <c r="I65" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[63] = new TableColDefEx("UseDESKeyOnly", typeof(Boolean), "USE_DES_KEY_ONLY","UAC");</v>
+        <f>CONCATENATE("collist[",F65,"] = new TableColDefEx(""",C65,""", typeof(",B65,"), """,H65,""",""",G65,""");")</f>
+        <v>collist[63] = new TableColDefEx("ObjectClass", typeof(String), "SchemaClassName","ObjClass");</v>
       </c>
       <c r="J65" t="str">
-        <f t="shared" si="1"/>
-        <v>[UseDESKeyOnly] [bit] NULL,</v>
+        <f>CONCATENATE("[",C65,"] [",A65,"](",D65,") ",E65,",")</f>
+        <v>[ObjectClass] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -9167,65 +9145,65 @@
         <v>83</v>
       </c>
       <c r="C66" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D66">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="E66" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F66" s="6">
         <v>64</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H66" s="15" t="s">
-        <v>179</v>
+        <v>59</v>
+      </c>
+      <c r="H66" t="s">
+        <v>138</v>
       </c>
       <c r="I66" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>collist[64] = new TableColDefEx("UserPrincipalName", typeof(String), "userprincipalname","Adprop");</v>
+        <f>CONCATENATE("collist[",F66,"] = new TableColDefEx(""",C66,""", typeof(",B66,"), """,H66,""",""",G66,""");")</f>
+        <v>collist[64] = new TableColDefEx("SID", typeof(String), "objectsid","SID");</v>
       </c>
       <c r="J66" t="str">
         <f>CONCATENATE("[",C66,"] [",A66,"](",D66,") ",E66,",")</f>
-        <v>[UserPrincipalName] [nvarchar](256) NULL,</v>
+        <v>[SID] [nvarchar](128) NOT NULL,</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="B67" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C67" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="E67" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F67" s="6">
         <v>65</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H67" s="15" t="s">
-        <v>146</v>
+        <v>172</v>
+      </c>
+      <c r="H67" t="s">
+        <v>71</v>
       </c>
       <c r="I67" s="1" t="str">
-        <f t="shared" ref="I67" si="2">CONCATENATE("collist[",F67,"] = new TableColDefEx(""",C67,""", typeof(",B67,"), """,H67,""",""",G67,""");")</f>
-        <v>collist[65] = new TableColDefEx("userAccountControl", typeof(Int32), "useraccountcontrol","Adprop");</v>
+        <f>CONCATENATE("collist[",F67,"] = new TableColDefEx(""",C67,""", typeof(",B67,"), """,H67,""",""",G67,""");")</f>
+        <v>collist[65] = new TableColDefEx("ObjectGUID", typeof(Guid), "Guid","ObjGuid");</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" si="1"/>
-        <v>[userAccountControl] [int] NULL,</v>
+        <f>CONCATENATE("[",C67,"] [",A67,"] ",E67,",")</f>
+        <v>[ObjectGUID] [uniqueidentifier] NOT NULL,</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J68"/>
+  <autoFilter ref="A1:J60"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -9235,8 +9213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10442,8 +10420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I42"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10514,7 +10492,7 @@
       <c r="G2" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" t="s">
         <v>127</v>
       </c>
       <c r="I2" s="1" t="str">
@@ -10548,7 +10526,7 @@
       <c r="G3" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" t="s">
         <v>155</v>
       </c>
       <c r="I3" s="1" t="str">
@@ -10582,7 +10560,7 @@
       <c r="G4" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" t="s">
         <v>120</v>
       </c>
       <c r="I4" s="1" t="str">
@@ -10616,7 +10594,7 @@
       <c r="G5" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" t="s">
         <v>131</v>
       </c>
       <c r="I5" s="1" t="str">
@@ -10752,7 +10730,7 @@
       <c r="G9" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" t="s">
         <v>142</v>
       </c>
       <c r="I9" s="1" t="str">
@@ -10783,7 +10761,7 @@
       <c r="G10" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" t="s">
         <v>161</v>
       </c>
       <c r="I10" s="1" t="str">
@@ -10814,7 +10792,7 @@
       <c r="G11" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" t="s">
         <v>166</v>
       </c>
       <c r="I11" s="1" t="str">
@@ -10845,7 +10823,7 @@
       <c r="G12" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" t="s">
         <v>103</v>
       </c>
       <c r="I12" s="1" t="str">
@@ -10876,7 +10854,7 @@
       <c r="G13" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" t="s">
         <v>163</v>
       </c>
       <c r="I13" s="1" t="str">
@@ -10907,7 +10885,7 @@
       <c r="G14" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" t="s">
         <v>104</v>
       </c>
       <c r="I14" s="1" t="str">
@@ -10938,7 +10916,7 @@
       <c r="G15" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" t="s">
         <v>164</v>
       </c>
       <c r="I15" s="1" t="str">
@@ -10969,7 +10947,7 @@
       <c r="G16" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="H16" t="s">
         <v>162</v>
       </c>
       <c r="I16" s="1" t="str">
@@ -11000,7 +10978,7 @@
       <c r="G17" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" t="s">
         <v>165</v>
       </c>
       <c r="I17" s="1" t="str">
@@ -11031,7 +11009,7 @@
       <c r="G18" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" t="s">
         <v>107</v>
       </c>
       <c r="I18" s="1" t="str">
@@ -11062,7 +11040,7 @@
       <c r="G19" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" t="s">
         <v>167</v>
       </c>
       <c r="I19" s="1" t="str">
@@ -11093,7 +11071,7 @@
       <c r="G20" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" t="s">
         <v>105</v>
       </c>
       <c r="I20" s="1" t="str">
@@ -11124,7 +11102,7 @@
       <c r="G21" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H21" t="s">
         <v>102</v>
       </c>
       <c r="I21" s="1" t="str">
@@ -11155,7 +11133,7 @@
       <c r="G22" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H22" t="s">
         <v>100</v>
       </c>
       <c r="I22" s="1" t="str">
@@ -11186,7 +11164,7 @@
       <c r="G23" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H23" s="17" t="s">
+      <c r="H23" t="s">
         <v>101</v>
       </c>
       <c r="I23" s="1" t="str">
@@ -11217,7 +11195,7 @@
       <c r="G24" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H24" t="s">
         <v>156</v>
       </c>
       <c r="I24" s="1" t="str">
@@ -11248,7 +11226,7 @@
       <c r="G25" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" t="s">
         <v>150</v>
       </c>
       <c r="I25" s="1" t="str">
@@ -11279,7 +11257,7 @@
       <c r="G26" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H26" t="s">
         <v>199</v>
       </c>
       <c r="I26" s="1" t="str">
@@ -11341,7 +11319,7 @@
       <c r="G28" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="H28" t="s">
         <v>149</v>
       </c>
       <c r="I28" s="1" t="str">
@@ -11372,7 +11350,7 @@
       <c r="G29" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H29" s="16" t="s">
+      <c r="H29" t="s">
         <v>168</v>
       </c>
       <c r="I29" s="1" t="str">
@@ -11403,7 +11381,7 @@
       <c r="G30" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="H30" t="s">
         <v>145</v>
       </c>
       <c r="I30" s="1" t="str">
@@ -11434,7 +11412,7 @@
       <c r="G31" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H31" s="15" t="s">
+      <c r="H31" t="s">
         <v>93</v>
       </c>
       <c r="I31" s="1" t="str">
@@ -11465,7 +11443,7 @@
       <c r="G32" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="H32" t="s">
         <v>94</v>
       </c>
       <c r="I32" s="1" t="str">
@@ -11499,7 +11477,7 @@
       <c r="G33" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H33" s="15" t="s">
+      <c r="H33" t="s">
         <v>152</v>
       </c>
       <c r="I33" s="1" t="str">
@@ -11533,7 +11511,7 @@
       <c r="G34" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H34" s="15" t="s">
+      <c r="H34" t="s">
         <v>141</v>
       </c>
       <c r="I34" s="1" t="str">
@@ -11567,7 +11545,7 @@
       <c r="G35" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H35" s="15" t="s">
+      <c r="H35" t="s">
         <v>140</v>
       </c>
       <c r="I35" s="1" t="str">
@@ -11601,7 +11579,7 @@
       <c r="G36" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H36" s="15" t="s">
+      <c r="H36" t="s">
         <v>153</v>
       </c>
       <c r="I36" s="1" t="str">
@@ -11635,7 +11613,7 @@
       <c r="G37" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H37" s="15" t="s">
+      <c r="H37" t="s">
         <v>137</v>
       </c>
       <c r="I37" s="1" t="str">
@@ -11666,7 +11644,7 @@
       <c r="G38" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H38" s="15" t="s">
+      <c r="H38" t="s">
         <v>146</v>
       </c>
       <c r="I38" s="1" t="str">
@@ -11700,7 +11678,7 @@
       <c r="G39" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H39" s="15" t="s">
+      <c r="H39" t="s">
         <v>139</v>
       </c>
       <c r="I39" s="1" t="str">
@@ -11734,7 +11712,7 @@
       <c r="G40" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="H40" s="15" t="s">
+      <c r="H40" t="s">
         <v>144</v>
       </c>
       <c r="I40" s="1" t="str">
@@ -11768,7 +11746,7 @@
       <c r="G41" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H41" s="15" t="s">
+      <c r="H41" t="s">
         <v>138</v>
       </c>
       <c r="I41" s="1" t="str">
@@ -11799,7 +11777,7 @@
       <c r="G42" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="H42" s="15" t="s">
+      <c r="H42" t="s">
         <v>71</v>
       </c>
       <c r="I42" s="1" t="str">
@@ -11822,8 +11800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11891,7 +11869,7 @@
       <c r="G2" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" t="s">
         <v>127</v>
       </c>
       <c r="I2" s="1" t="str">
@@ -11925,7 +11903,7 @@
       <c r="G3" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" t="s">
         <v>143</v>
       </c>
       <c r="I3" s="1" t="str">
@@ -11959,7 +11937,7 @@
       <c r="G4" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" t="s">
         <v>143</v>
       </c>
       <c r="I4" s="1" t="str">
@@ -11982,7 +11960,7 @@
         <v>18</v>
       </c>
       <c r="D5">
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="E5" t="s">
         <v>115</v>
@@ -11993,7 +11971,7 @@
       <c r="G5" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" t="s">
         <v>120</v>
       </c>
       <c r="I5" s="1" t="str">
@@ -12002,7 +11980,7 @@
       </c>
       <c r="J5" t="str">
         <f>CONCATENATE("[",C5,"] [",A5,"](",D5,") ",E5,",")</f>
-        <v>[Description] [nvarchar](256) NULL,</v>
+        <v>[Description] [nvarchar](512) NULL,</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -12027,7 +12005,7 @@
       <c r="G6" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" t="s">
         <v>123</v>
       </c>
       <c r="I6" s="1" t="str">
@@ -12061,7 +12039,7 @@
       <c r="G7" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" t="s">
         <v>142</v>
       </c>
       <c r="I7" s="1" t="str">
@@ -12095,7 +12073,7 @@
       <c r="G8" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" t="s">
         <v>140</v>
       </c>
       <c r="I8" s="1" t="str">
@@ -12129,7 +12107,7 @@
       <c r="G9" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" t="s">
         <v>141</v>
       </c>
       <c r="I9" s="1" t="str">
@@ -12160,7 +12138,7 @@
       <c r="G10" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" t="s">
         <v>93</v>
       </c>
       <c r="I10" s="1" t="str">
@@ -12191,7 +12169,7 @@
       <c r="G11" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" t="s">
         <v>94</v>
       </c>
       <c r="I11" s="1" t="str">
@@ -12225,7 +12203,7 @@
       <c r="G12" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" t="s">
         <v>137</v>
       </c>
       <c r="I12" s="1" t="str">
@@ -12259,7 +12237,7 @@
       <c r="G13" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" t="s">
         <v>139</v>
       </c>
       <c r="I13" s="1" t="str">
@@ -12293,7 +12271,7 @@
       <c r="G14" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" t="s">
         <v>144</v>
       </c>
       <c r="I14" s="1" t="str">
@@ -12327,7 +12305,7 @@
       <c r="G15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" t="s">
         <v>138</v>
       </c>
       <c r="I15" s="1" t="str">
@@ -12358,7 +12336,7 @@
       <c r="G16" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="H16" t="s">
         <v>71</v>
       </c>
       <c r="I16" s="1" t="str">

</xml_diff>